<commit_message>
CIERRE 26 aGO 22
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL  ARCHIVO   2 0 2 2/CENTRAL #08  AGOSTO 2022/BALANCE    ZAVALETA   AGOSTO   2022.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL  ARCHIVO   2 0 2 2/CENTRAL #08  AGOSTO 2022/BALANCE    ZAVALETA   AGOSTO   2022.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3690" yWindow="0" windowWidth="16605" windowHeight="10920" firstSheet="20" activeTab="22"/>
+    <workbookView xWindow="3690" yWindow="0" windowWidth="16605" windowHeight="10920" firstSheet="20" activeTab="21"/>
   </bookViews>
   <sheets>
     <sheet name="OCTUBRE      2 0 2 1     " sheetId="1" r:id="rId1"/>
@@ -830,7 +830,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2179" uniqueCount="1184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2180" uniqueCount="1185">
   <si>
     <t>COMPRAS</t>
   </si>
@@ -4416,6 +4416,9 @@
   </si>
   <si>
     <t>07874 D</t>
+  </si>
+  <si>
+    <t>27-Jul-22--26-Agos-22</t>
   </si>
 </sst>
 </file>
@@ -6558,7 +6561,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="884">
+  <cellXfs count="887">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -8061,6 +8064,39 @@
     <xf numFmtId="164" fontId="33" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -8133,76 +8169,10 @@
     <xf numFmtId="44" fontId="12" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="1" fontId="43" fillId="6" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="43" fillId="6" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="7" fontId="33" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="33" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="11" fillId="14" borderId="65" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="11" fillId="14" borderId="41" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="33" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="7" fontId="11" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="44" fontId="13" fillId="0" borderId="57" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -8246,6 +8216,39 @@
     </xf>
     <xf numFmtId="44" fontId="41" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="13" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="7" fontId="33" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="33" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="11" fillId="14" borderId="65" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="11" fillId="14" borderId="41" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="33" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="7" fontId="11" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="44" fontId="3" fillId="3" borderId="74" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -8457,6 +8460,15 @@
     <xf numFmtId="165" fontId="11" fillId="0" borderId="96" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="44" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="11" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="44" fontId="11" fillId="14" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -8471,15 +8483,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="11" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="11" fillId="18" borderId="74" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -8499,6 +8502,11 @@
     <xf numFmtId="49" fontId="11" fillId="23" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="165" fontId="3" fillId="26" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="15" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="3" fillId="15" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
@@ -8508,6 +8516,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF00FF00"/>
       <color rgb="FFCC99FF"/>
       <color rgb="FFFF00FF"/>
       <color rgb="FF99CCFF"/>
@@ -8517,7 +8526,6 @@
       <color rgb="FF00FF99"/>
       <color rgb="FFCCFF66"/>
       <color rgb="FF990033"/>
-      <color rgb="FFCC3399"/>
     </mruColors>
   </colors>
   <extLst>
@@ -10737,55 +10745,6 @@
         </a:fillRef>
         <a:effectRef idx="2">
           <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing15.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>485775</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>323850</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="2" name="Conector recto 1"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1381125" y="5838825"/>
-          <a:ext cx="3857625" cy="19050"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="3">
-          <a:schemeClr val="accent2"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent2"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="accent2"/>
         </a:effectRef>
         <a:fontRef idx="minor">
           <a:schemeClr val="tx1"/>
@@ -13862,23 +13821,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="762"/>
-      <c r="C1" s="764" t="s">
+      <c r="B1" s="738"/>
+      <c r="C1" s="740" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="765"/>
-      <c r="E1" s="765"/>
-      <c r="F1" s="765"/>
-      <c r="G1" s="765"/>
-      <c r="H1" s="765"/>
-      <c r="I1" s="765"/>
-      <c r="J1" s="765"/>
-      <c r="K1" s="765"/>
-      <c r="L1" s="765"/>
-      <c r="M1" s="765"/>
+      <c r="D1" s="741"/>
+      <c r="E1" s="741"/>
+      <c r="F1" s="741"/>
+      <c r="G1" s="741"/>
+      <c r="H1" s="741"/>
+      <c r="I1" s="741"/>
+      <c r="J1" s="741"/>
+      <c r="K1" s="741"/>
+      <c r="L1" s="741"/>
+      <c r="M1" s="741"/>
     </row>
     <row r="2" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="763"/>
+      <c r="B2" s="739"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -13888,17 +13847,17 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:19" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="766" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="767"/>
+      <c r="B3" s="742" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="743"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="768" t="s">
+      <c r="H3" s="744" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="768"/>
+      <c r="I3" s="744"/>
       <c r="K3" s="165"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
@@ -13912,14 +13871,14 @@
         <v>0</v>
       </c>
       <c r="D4" s="18"/>
-      <c r="E4" s="769" t="s">
+      <c r="E4" s="745" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="770"/>
-      <c r="H4" s="771" t="s">
+      <c r="F4" s="746"/>
+      <c r="H4" s="747" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="772"/>
+      <c r="I4" s="748"/>
       <c r="J4" s="19"/>
       <c r="K4" s="166"/>
       <c r="L4" s="20"/>
@@ -13929,10 +13888,10 @@
       <c r="N4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="743" t="s">
+      <c r="P4" s="754" t="s">
         <v>6</v>
       </c>
-      <c r="Q4" s="744"/>
+      <c r="Q4" s="755"/>
     </row>
     <row r="5" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="23" t="s">
@@ -15373,11 +15332,11 @@
       <c r="J39" s="60"/>
       <c r="K39" s="177"/>
       <c r="L39" s="61"/>
-      <c r="M39" s="745">
+      <c r="M39" s="756">
         <f>SUM(M5:M38)</f>
         <v>247061</v>
       </c>
-      <c r="N39" s="747">
+      <c r="N39" s="758">
         <f>SUM(N5:N38)</f>
         <v>172863</v>
       </c>
@@ -15403,8 +15362,8 @@
       <c r="J40" s="60"/>
       <c r="K40" s="41"/>
       <c r="L40" s="61"/>
-      <c r="M40" s="746"/>
-      <c r="N40" s="748"/>
+      <c r="M40" s="757"/>
+      <c r="N40" s="759"/>
       <c r="P40" s="34"/>
       <c r="Q40" s="9"/>
     </row>
@@ -15619,29 +15578,29 @@
       <c r="A52" s="98"/>
       <c r="B52" s="99"/>
       <c r="C52" s="1"/>
-      <c r="H52" s="749" t="s">
+      <c r="H52" s="760" t="s">
         <v>11</v>
       </c>
-      <c r="I52" s="750"/>
+      <c r="I52" s="761"/>
       <c r="J52" s="100"/>
-      <c r="K52" s="751">
+      <c r="K52" s="762">
         <f>I50+L50</f>
         <v>53873.49</v>
       </c>
-      <c r="L52" s="752"/>
-      <c r="M52" s="753">
+      <c r="L52" s="763"/>
+      <c r="M52" s="764">
         <f>N39+M39</f>
         <v>419924</v>
       </c>
-      <c r="N52" s="754"/>
+      <c r="N52" s="765"/>
       <c r="P52" s="34"/>
       <c r="Q52" s="9"/>
     </row>
     <row r="53" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D53" s="755" t="s">
+      <c r="D53" s="766" t="s">
         <v>12</v>
       </c>
-      <c r="E53" s="755"/>
+      <c r="E53" s="766"/>
       <c r="F53" s="101">
         <f>F50-K52-C50</f>
         <v>471038.61</v>
@@ -15652,22 +15611,22 @@
       <c r="Q53" s="9"/>
     </row>
     <row r="54" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D54" s="755" t="s">
+      <c r="D54" s="766" t="s">
         <v>95</v>
       </c>
-      <c r="E54" s="755"/>
+      <c r="E54" s="766"/>
       <c r="F54" s="96">
         <v>-549976.4</v>
       </c>
-      <c r="I54" s="756" t="s">
+      <c r="I54" s="767" t="s">
         <v>13</v>
       </c>
-      <c r="J54" s="757"/>
-      <c r="K54" s="758">
+      <c r="J54" s="768"/>
+      <c r="K54" s="769">
         <f>F56+F57+F58</f>
         <v>-24577.400000000023</v>
       </c>
-      <c r="L54" s="759"/>
+      <c r="L54" s="770"/>
       <c r="P54" s="34"/>
       <c r="Q54" s="9"/>
     </row>
@@ -15700,11 +15659,11 @@
         <v>15</v>
       </c>
       <c r="J56" s="109"/>
-      <c r="K56" s="760">
+      <c r="K56" s="771">
         <f>-C4</f>
         <v>0</v>
       </c>
-      <c r="L56" s="761"/>
+      <c r="L56" s="772"/>
     </row>
     <row r="57" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="110" t="s">
@@ -15721,22 +15680,22 @@
       <c r="C58" s="112">
         <v>44507</v>
       </c>
-      <c r="D58" s="738" t="s">
+      <c r="D58" s="749" t="s">
         <v>18</v>
       </c>
-      <c r="E58" s="739"/>
+      <c r="E58" s="750"/>
       <c r="F58" s="113">
         <v>567389.35</v>
       </c>
-      <c r="I58" s="740" t="s">
+      <c r="I58" s="751" t="s">
         <v>97</v>
       </c>
-      <c r="J58" s="741"/>
-      <c r="K58" s="742">
+      <c r="J58" s="752"/>
+      <c r="K58" s="753">
         <f>K54+K56</f>
         <v>-24577.400000000023</v>
       </c>
-      <c r="L58" s="742"/>
+      <c r="L58" s="753"/>
     </row>
     <row r="59" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C59" s="114"/>
@@ -15880,12 +15839,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
     <mergeCell ref="D58:E58"/>
     <mergeCell ref="I58:J58"/>
     <mergeCell ref="K58:L58"/>
@@ -15900,6 +15853,12 @@
     <mergeCell ref="I54:J54"/>
     <mergeCell ref="K54:L54"/>
     <mergeCell ref="K56:L56"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
   </mergeCells>
   <pageMargins left="0.39370078740157483" right="0.15748031496062992" top="0.35433070866141736" bottom="0.31496062992125984" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="75" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -18758,7 +18717,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="762"/>
+      <c r="B1" s="738"/>
       <c r="C1" s="804" t="s">
         <v>451</v>
       </c>
@@ -18774,7 +18733,7 @@
       <c r="M1" s="805"/>
     </row>
     <row r="2" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="763"/>
+      <c r="B2" s="739"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -18784,21 +18743,21 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:25" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="766" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="767"/>
+      <c r="B3" s="742" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="743"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="768" t="s">
+      <c r="H3" s="744" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="768"/>
+      <c r="I3" s="744"/>
       <c r="K3" s="165"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
-      <c r="P3" s="792" t="s">
+      <c r="P3" s="781" t="s">
         <v>6</v>
       </c>
       <c r="R3" s="802" t="s">
@@ -18816,14 +18775,14 @@
       <c r="D4" s="18">
         <v>44619</v>
       </c>
-      <c r="E4" s="769" t="s">
+      <c r="E4" s="745" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="770"/>
-      <c r="H4" s="771" t="s">
+      <c r="F4" s="746"/>
+      <c r="H4" s="747" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="772"/>
+      <c r="I4" s="748"/>
       <c r="J4" s="19"/>
       <c r="K4" s="166"/>
       <c r="L4" s="20"/>
@@ -18833,15 +18792,15 @@
       <c r="N4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="793"/>
+      <c r="P4" s="782"/>
       <c r="Q4" s="322" t="s">
         <v>217</v>
       </c>
       <c r="R4" s="803"/>
-      <c r="W4" s="775" t="s">
+      <c r="W4" s="791" t="s">
         <v>124</v>
       </c>
-      <c r="X4" s="775"/>
+      <c r="X4" s="791"/>
       <c r="Y4" s="227"/>
     </row>
     <row r="5" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -18892,8 +18851,8 @@
         <v>0</v>
       </c>
       <c r="S5" s="324"/>
-      <c r="W5" s="775"/>
-      <c r="X5" s="775"/>
+      <c r="W5" s="791"/>
+      <c r="X5" s="791"/>
       <c r="Y5" s="233"/>
     </row>
     <row r="6" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -19656,7 +19615,7 @@
         <v>0</v>
       </c>
       <c r="S19" s="147"/>
-      <c r="W19" s="779">
+      <c r="W19" s="795">
         <f>SUM(W6:W18)</f>
         <v>0</v>
       </c>
@@ -19708,7 +19667,7 @@
         <v>0</v>
       </c>
       <c r="S20" s="147"/>
-      <c r="W20" s="780"/>
+      <c r="W20" s="796"/>
       <c r="X20" s="268"/>
       <c r="Y20" s="233"/>
     </row>
@@ -19757,8 +19716,8 @@
         <v>0</v>
       </c>
       <c r="S21" s="147"/>
-      <c r="W21" s="781"/>
-      <c r="X21" s="781"/>
+      <c r="W21" s="797"/>
+      <c r="X21" s="797"/>
       <c r="Y21" s="233"/>
       <c r="Z21" s="128"/>
     </row>
@@ -19858,8 +19817,8 @@
         <v>0</v>
       </c>
       <c r="S23" s="147"/>
-      <c r="W23" s="782"/>
-      <c r="X23" s="782"/>
+      <c r="W23" s="798"/>
+      <c r="X23" s="798"/>
       <c r="Y23" s="233"/>
       <c r="Z23" s="128"/>
     </row>
@@ -19914,8 +19873,8 @@
         <v>0</v>
       </c>
       <c r="S24" s="147"/>
-      <c r="W24" s="782"/>
-      <c r="X24" s="782"/>
+      <c r="W24" s="798"/>
+      <c r="X24" s="798"/>
       <c r="Y24" s="233"/>
       <c r="Z24" s="128"/>
     </row>
@@ -19963,8 +19922,8 @@
       <c r="R25" s="319">
         <v>0</v>
       </c>
-      <c r="W25" s="783"/>
-      <c r="X25" s="783"/>
+      <c r="W25" s="799"/>
+      <c r="X25" s="799"/>
       <c r="Y25" s="233"/>
       <c r="Z25" s="128"/>
     </row>
@@ -20013,8 +19972,8 @@
       <c r="R26" s="319">
         <v>0</v>
       </c>
-      <c r="W26" s="783"/>
-      <c r="X26" s="783"/>
+      <c r="W26" s="799"/>
+      <c r="X26" s="799"/>
       <c r="Y26" s="233"/>
       <c r="Z26" s="128"/>
     </row>
@@ -20062,9 +20021,9 @@
       <c r="R27" s="388">
         <v>170</v>
       </c>
-      <c r="W27" s="776"/>
-      <c r="X27" s="777"/>
-      <c r="Y27" s="778"/>
+      <c r="W27" s="792"/>
+      <c r="X27" s="793"/>
+      <c r="Y27" s="794"/>
       <c r="Z27" s="128"/>
     </row>
     <row r="28" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -20112,9 +20071,9 @@
       <c r="R28" s="388">
         <v>37374.36</v>
       </c>
-      <c r="W28" s="777"/>
-      <c r="X28" s="777"/>
-      <c r="Y28" s="778"/>
+      <c r="W28" s="793"/>
+      <c r="X28" s="793"/>
+      <c r="Y28" s="794"/>
       <c r="Z28" s="128"/>
     </row>
     <row r="29" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -20446,11 +20405,11 @@
       <c r="J36" s="266"/>
       <c r="K36" s="250"/>
       <c r="L36" s="44"/>
-      <c r="M36" s="794">
+      <c r="M36" s="783">
         <f>SUM(M5:M35)</f>
         <v>2220612.02</v>
       </c>
-      <c r="N36" s="796">
+      <c r="N36" s="785">
         <f>SUM(N5:N35)</f>
         <v>833865</v>
       </c>
@@ -20483,8 +20442,8 @@
       <c r="J37" s="60"/>
       <c r="K37" s="41"/>
       <c r="L37" s="61"/>
-      <c r="M37" s="795"/>
-      <c r="N37" s="797"/>
+      <c r="M37" s="784"/>
+      <c r="N37" s="786"/>
       <c r="O37" s="276"/>
       <c r="P37" s="277">
         <v>0</v>
@@ -21171,26 +21130,26 @@
       <c r="A68" s="98"/>
       <c r="B68" s="99"/>
       <c r="C68" s="1"/>
-      <c r="H68" s="749" t="s">
+      <c r="H68" s="760" t="s">
         <v>11</v>
       </c>
-      <c r="I68" s="750"/>
+      <c r="I68" s="761"/>
       <c r="J68" s="100"/>
-      <c r="K68" s="751">
+      <c r="K68" s="762">
         <f>I66+L66</f>
         <v>314868.39999999997</v>
       </c>
-      <c r="L68" s="784"/>
+      <c r="L68" s="789"/>
       <c r="M68" s="272"/>
       <c r="N68" s="272"/>
       <c r="P68" s="34"/>
       <c r="Q68" s="13"/>
     </row>
     <row r="69" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D69" s="755" t="s">
+      <c r="D69" s="766" t="s">
         <v>12</v>
       </c>
-      <c r="E69" s="755"/>
+      <c r="E69" s="766"/>
       <c r="F69" s="312">
         <f>F66-K68-C66</f>
         <v>1594593.8500000003</v>
@@ -21199,22 +21158,22 @@
       <c r="J69" s="103"/>
     </row>
     <row r="70" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D70" s="785" t="s">
+      <c r="D70" s="790" t="s">
         <v>95</v>
       </c>
-      <c r="E70" s="785"/>
+      <c r="E70" s="790"/>
       <c r="F70" s="111">
         <v>-1360260.32</v>
       </c>
-      <c r="I70" s="756" t="s">
+      <c r="I70" s="767" t="s">
         <v>13</v>
       </c>
-      <c r="J70" s="757"/>
-      <c r="K70" s="758">
+      <c r="J70" s="768"/>
+      <c r="K70" s="769">
         <f>F72+F73+F74</f>
         <v>1938640.11</v>
       </c>
-      <c r="L70" s="758"/>
+      <c r="L70" s="769"/>
       <c r="M70" s="404"/>
       <c r="N70" s="404"/>
       <c r="O70" s="404"/>
@@ -21255,11 +21214,11 @@
         <v>15</v>
       </c>
       <c r="J72" s="109"/>
-      <c r="K72" s="760">
+      <c r="K72" s="771">
         <f>-C4</f>
         <v>-1266568.45</v>
       </c>
-      <c r="L72" s="761"/>
+      <c r="L72" s="772"/>
     </row>
     <row r="73" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D73" s="110" t="s">
@@ -21276,22 +21235,22 @@
       <c r="C74" s="112">
         <v>44647</v>
       </c>
-      <c r="D74" s="738" t="s">
+      <c r="D74" s="749" t="s">
         <v>18</v>
       </c>
-      <c r="E74" s="739"/>
+      <c r="E74" s="750"/>
       <c r="F74" s="113">
         <v>1792817.68</v>
       </c>
-      <c r="I74" s="740" t="s">
+      <c r="I74" s="751" t="s">
         <v>198</v>
       </c>
-      <c r="J74" s="741"/>
-      <c r="K74" s="742">
+      <c r="J74" s="752"/>
+      <c r="K74" s="753">
         <f>K70+K72</f>
         <v>672071.66000000015</v>
       </c>
-      <c r="L74" s="742"/>
+      <c r="L74" s="753"/>
     </row>
     <row r="75" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C75" s="114"/>
@@ -21438,21 +21397,6 @@
     <sortCondition ref="B34:B42"/>
   </sortState>
   <mergeCells count="30">
-    <mergeCell ref="D74:E74"/>
-    <mergeCell ref="I74:J74"/>
-    <mergeCell ref="K74:L74"/>
-    <mergeCell ref="H68:I68"/>
-    <mergeCell ref="K68:L68"/>
-    <mergeCell ref="D69:E69"/>
-    <mergeCell ref="D70:E70"/>
-    <mergeCell ref="I70:J70"/>
-    <mergeCell ref="K70:L70"/>
-    <mergeCell ref="Y27:Y28"/>
-    <mergeCell ref="M36:M37"/>
-    <mergeCell ref="N36:N37"/>
-    <mergeCell ref="Q36:Q37"/>
-    <mergeCell ref="K72:L72"/>
-    <mergeCell ref="M39:N39"/>
     <mergeCell ref="W26:X26"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="W27:X28"/>
@@ -21468,6 +21412,21 @@
     <mergeCell ref="W21:X21"/>
     <mergeCell ref="W23:X24"/>
     <mergeCell ref="W25:X25"/>
+    <mergeCell ref="Y27:Y28"/>
+    <mergeCell ref="M36:M37"/>
+    <mergeCell ref="N36:N37"/>
+    <mergeCell ref="Q36:Q37"/>
+    <mergeCell ref="K72:L72"/>
+    <mergeCell ref="M39:N39"/>
+    <mergeCell ref="D74:E74"/>
+    <mergeCell ref="I74:J74"/>
+    <mergeCell ref="K74:L74"/>
+    <mergeCell ref="H68:I68"/>
+    <mergeCell ref="K68:L68"/>
+    <mergeCell ref="D69:E69"/>
+    <mergeCell ref="D70:E70"/>
+    <mergeCell ref="I70:J70"/>
+    <mergeCell ref="K70:L70"/>
   </mergeCells>
   <pageMargins left="0.27559055118110237" right="0.15748031496062992" top="0.39370078740157483" bottom="0.27559055118110237" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="80" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -24080,7 +24039,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="762"/>
+      <c r="B1" s="738"/>
       <c r="C1" s="804" t="s">
         <v>620</v>
       </c>
@@ -24096,7 +24055,7 @@
       <c r="M1" s="805"/>
     </row>
     <row r="2" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="763"/>
+      <c r="B2" s="739"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -24106,21 +24065,21 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:25" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="766" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="767"/>
+      <c r="B3" s="742" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="743"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="768" t="s">
+      <c r="H3" s="744" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="768"/>
+      <c r="I3" s="744"/>
       <c r="K3" s="165"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
-      <c r="P3" s="792" t="s">
+      <c r="P3" s="781" t="s">
         <v>6</v>
       </c>
       <c r="R3" s="802" t="s">
@@ -24138,14 +24097,14 @@
       <c r="D4" s="18">
         <v>44647</v>
       </c>
-      <c r="E4" s="769" t="s">
+      <c r="E4" s="745" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="770"/>
-      <c r="H4" s="771" t="s">
+      <c r="F4" s="746"/>
+      <c r="H4" s="747" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="772"/>
+      <c r="I4" s="748"/>
       <c r="J4" s="19"/>
       <c r="K4" s="166"/>
       <c r="L4" s="20"/>
@@ -24155,15 +24114,15 @@
       <c r="N4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="793"/>
+      <c r="P4" s="782"/>
       <c r="Q4" s="322" t="s">
         <v>217</v>
       </c>
       <c r="R4" s="803"/>
-      <c r="W4" s="775" t="s">
+      <c r="W4" s="791" t="s">
         <v>124</v>
       </c>
-      <c r="X4" s="775"/>
+      <c r="X4" s="791"/>
       <c r="Y4" s="227"/>
     </row>
     <row r="5" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -24214,8 +24173,8 @@
         <v>0</v>
       </c>
       <c r="S5" s="324"/>
-      <c r="W5" s="775"/>
-      <c r="X5" s="775"/>
+      <c r="W5" s="791"/>
+      <c r="X5" s="791"/>
       <c r="Y5" s="233"/>
     </row>
     <row r="6" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -24974,7 +24933,7 @@
         <v>0</v>
       </c>
       <c r="S19" s="147"/>
-      <c r="W19" s="779">
+      <c r="W19" s="795">
         <f>SUM(W6:W18)</f>
         <v>0</v>
       </c>
@@ -25026,7 +24985,7 @@
         <v>0</v>
       </c>
       <c r="S20" s="147"/>
-      <c r="W20" s="780"/>
+      <c r="W20" s="796"/>
       <c r="X20" s="268"/>
       <c r="Y20" s="233"/>
     </row>
@@ -25075,8 +25034,8 @@
         <v>0</v>
       </c>
       <c r="S21" s="147"/>
-      <c r="W21" s="781"/>
-      <c r="X21" s="781"/>
+      <c r="W21" s="797"/>
+      <c r="X21" s="797"/>
       <c r="Y21" s="233"/>
       <c r="Z21" s="128"/>
     </row>
@@ -25173,8 +25132,8 @@
         <v>0</v>
       </c>
       <c r="S23" s="147"/>
-      <c r="W23" s="782"/>
-      <c r="X23" s="782"/>
+      <c r="W23" s="798"/>
+      <c r="X23" s="798"/>
       <c r="Y23" s="233"/>
       <c r="Z23" s="128"/>
     </row>
@@ -25229,8 +25188,8 @@
         <v>642</v>
       </c>
       <c r="S24" s="147"/>
-      <c r="W24" s="782"/>
-      <c r="X24" s="782"/>
+      <c r="W24" s="798"/>
+      <c r="X24" s="798"/>
       <c r="Y24" s="233"/>
       <c r="Z24" s="128"/>
     </row>
@@ -25276,8 +25235,8 @@
       <c r="R25" s="319">
         <v>0</v>
       </c>
-      <c r="W25" s="783"/>
-      <c r="X25" s="783"/>
+      <c r="W25" s="799"/>
+      <c r="X25" s="799"/>
       <c r="Y25" s="233"/>
       <c r="Z25" s="128"/>
     </row>
@@ -25328,8 +25287,8 @@
       <c r="R26" s="388">
         <v>73524.61</v>
       </c>
-      <c r="W26" s="783"/>
-      <c r="X26" s="783"/>
+      <c r="W26" s="799"/>
+      <c r="X26" s="799"/>
       <c r="Y26" s="233"/>
       <c r="Z26" s="128"/>
     </row>
@@ -25380,9 +25339,9 @@
       <c r="R27" s="319">
         <v>0</v>
       </c>
-      <c r="W27" s="776"/>
-      <c r="X27" s="777"/>
-      <c r="Y27" s="778"/>
+      <c r="W27" s="792"/>
+      <c r="X27" s="793"/>
+      <c r="Y27" s="794"/>
       <c r="Z27" s="128"/>
     </row>
     <row r="28" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -25432,9 +25391,9 @@
       <c r="R28" s="319">
         <v>0</v>
       </c>
-      <c r="W28" s="777"/>
-      <c r="X28" s="777"/>
-      <c r="Y28" s="778"/>
+      <c r="W28" s="793"/>
+      <c r="X28" s="793"/>
+      <c r="Y28" s="794"/>
       <c r="Z28" s="128"/>
     </row>
     <row r="29" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -26038,11 +25997,11 @@
       <c r="L41" s="624">
         <v>15798.5</v>
       </c>
-      <c r="M41" s="794">
+      <c r="M41" s="783">
         <f>SUM(M5:M40)</f>
         <v>2479367.6100000003</v>
       </c>
-      <c r="N41" s="794">
+      <c r="N41" s="783">
         <f>SUM(N5:N40)</f>
         <v>1195667</v>
       </c>
@@ -26080,8 +26039,8 @@
       <c r="L42" s="627">
         <v>15298.5</v>
       </c>
-      <c r="M42" s="795"/>
-      <c r="N42" s="795"/>
+      <c r="M42" s="784"/>
+      <c r="N42" s="784"/>
       <c r="P42" s="34"/>
       <c r="Q42" s="849"/>
     </row>
@@ -26768,26 +26727,26 @@
       <c r="A70" s="98"/>
       <c r="B70" s="99"/>
       <c r="C70" s="1"/>
-      <c r="H70" s="749" t="s">
+      <c r="H70" s="760" t="s">
         <v>11</v>
       </c>
-      <c r="I70" s="750"/>
+      <c r="I70" s="761"/>
       <c r="J70" s="100"/>
-      <c r="K70" s="751">
+      <c r="K70" s="762">
         <f>I68+L68</f>
         <v>428155.54000000004</v>
       </c>
-      <c r="L70" s="784"/>
+      <c r="L70" s="789"/>
       <c r="M70" s="272"/>
       <c r="N70" s="272"/>
       <c r="P70" s="34"/>
       <c r="Q70" s="13"/>
     </row>
     <row r="71" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D71" s="755" t="s">
+      <c r="D71" s="766" t="s">
         <v>12</v>
       </c>
-      <c r="E71" s="755"/>
+      <c r="E71" s="766"/>
       <c r="F71" s="312">
         <f>F68-K70-C68</f>
         <v>1631087.67</v>
@@ -26797,22 +26756,22 @@
       <c r="P71" s="34"/>
     </row>
     <row r="72" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D72" s="785" t="s">
+      <c r="D72" s="790" t="s">
         <v>95</v>
       </c>
-      <c r="E72" s="785"/>
+      <c r="E72" s="790"/>
       <c r="F72" s="111">
         <v>-1884975.46</v>
       </c>
-      <c r="I72" s="756" t="s">
+      <c r="I72" s="767" t="s">
         <v>13</v>
       </c>
-      <c r="J72" s="757"/>
-      <c r="K72" s="758">
+      <c r="J72" s="768"/>
+      <c r="K72" s="769">
         <f>F74+F75+F76</f>
         <v>1777829.89</v>
       </c>
-      <c r="L72" s="758"/>
+      <c r="L72" s="769"/>
       <c r="M72" s="404"/>
       <c r="N72" s="404"/>
       <c r="O72" s="404"/>
@@ -26853,11 +26812,11 @@
         <v>15</v>
       </c>
       <c r="J74" s="109"/>
-      <c r="K74" s="760">
+      <c r="K74" s="771">
         <f>-C4</f>
         <v>-1792817.68</v>
       </c>
-      <c r="L74" s="761"/>
+      <c r="L74" s="772"/>
       <c r="P74" s="34"/>
     </row>
     <row r="75" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -26876,22 +26835,22 @@
       <c r="C76" s="112">
         <v>44682</v>
       </c>
-      <c r="D76" s="738" t="s">
+      <c r="D76" s="749" t="s">
         <v>18</v>
       </c>
-      <c r="E76" s="739"/>
+      <c r="E76" s="750"/>
       <c r="F76" s="113">
         <v>2112071.92</v>
       </c>
-      <c r="I76" s="740" t="s">
+      <c r="I76" s="751" t="s">
         <v>854</v>
       </c>
-      <c r="J76" s="741"/>
-      <c r="K76" s="742">
+      <c r="J76" s="752"/>
+      <c r="K76" s="753">
         <f>K72+K74</f>
         <v>-14987.790000000037</v>
       </c>
-      <c r="L76" s="742"/>
+      <c r="L76" s="753"/>
       <c r="P76" s="34"/>
     </row>
     <row r="77" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
@@ -27051,21 +27010,6 @@
     <sortCondition ref="J47:J67"/>
   </sortState>
   <mergeCells count="30">
-    <mergeCell ref="D76:E76"/>
-    <mergeCell ref="I76:J76"/>
-    <mergeCell ref="K76:L76"/>
-    <mergeCell ref="H70:I70"/>
-    <mergeCell ref="K70:L70"/>
-    <mergeCell ref="D71:E71"/>
-    <mergeCell ref="D72:E72"/>
-    <mergeCell ref="I72:J72"/>
-    <mergeCell ref="K72:L72"/>
-    <mergeCell ref="Y27:Y28"/>
-    <mergeCell ref="M41:M42"/>
-    <mergeCell ref="N41:N42"/>
-    <mergeCell ref="Q41:Q42"/>
-    <mergeCell ref="K74:L74"/>
-    <mergeCell ref="M45:N45"/>
     <mergeCell ref="W26:X26"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="W27:X28"/>
@@ -27081,6 +27025,21 @@
     <mergeCell ref="W21:X21"/>
     <mergeCell ref="W23:X24"/>
     <mergeCell ref="W25:X25"/>
+    <mergeCell ref="Y27:Y28"/>
+    <mergeCell ref="M41:M42"/>
+    <mergeCell ref="N41:N42"/>
+    <mergeCell ref="Q41:Q42"/>
+    <mergeCell ref="K74:L74"/>
+    <mergeCell ref="M45:N45"/>
+    <mergeCell ref="D76:E76"/>
+    <mergeCell ref="I76:J76"/>
+    <mergeCell ref="K76:L76"/>
+    <mergeCell ref="H70:I70"/>
+    <mergeCell ref="K70:L70"/>
+    <mergeCell ref="D71:E71"/>
+    <mergeCell ref="D72:E72"/>
+    <mergeCell ref="I72:J72"/>
+    <mergeCell ref="K72:L72"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.39370078740157483" bottom="0.35433070866141736" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="85" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -30538,7 +30497,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="762"/>
+      <c r="B1" s="738"/>
       <c r="C1" s="804" t="s">
         <v>754</v>
       </c>
@@ -30554,7 +30513,7 @@
       <c r="M1" s="805"/>
     </row>
     <row r="2" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="763"/>
+      <c r="B2" s="739"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -30564,21 +30523,21 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:25" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="766" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="767"/>
+      <c r="B3" s="742" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="743"/>
       <c r="D3" s="10"/>
       <c r="E3" s="553"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="768" t="s">
+      <c r="H3" s="744" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="768"/>
+      <c r="I3" s="744"/>
       <c r="K3" s="165"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
-      <c r="P3" s="792" t="s">
+      <c r="P3" s="781" t="s">
         <v>6</v>
       </c>
       <c r="R3" s="802" t="s">
@@ -30600,14 +30559,14 @@
       <c r="D4" s="18">
         <v>44682</v>
       </c>
-      <c r="E4" s="769" t="s">
+      <c r="E4" s="745" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="770"/>
-      <c r="H4" s="771" t="s">
+      <c r="F4" s="746"/>
+      <c r="H4" s="747" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="772"/>
+      <c r="I4" s="748"/>
       <c r="J4" s="556"/>
       <c r="K4" s="562"/>
       <c r="L4" s="563"/>
@@ -30617,15 +30576,15 @@
       <c r="N4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="793"/>
+      <c r="P4" s="782"/>
       <c r="Q4" s="322" t="s">
         <v>217</v>
       </c>
       <c r="R4" s="803"/>
       <c r="U4" s="34"/>
       <c r="V4" s="128"/>
-      <c r="W4" s="876"/>
-      <c r="X4" s="876"/>
+      <c r="W4" s="870"/>
+      <c r="X4" s="870"/>
       <c r="Y4" s="227"/>
     </row>
     <row r="5" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -30679,8 +30638,8 @@
       <c r="S5" s="324"/>
       <c r="U5" s="34"/>
       <c r="V5" s="128"/>
-      <c r="W5" s="876"/>
-      <c r="X5" s="876"/>
+      <c r="W5" s="870"/>
+      <c r="X5" s="870"/>
       <c r="Y5" s="233"/>
     </row>
     <row r="6" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -31446,7 +31405,7 @@
       <c r="S19" s="147"/>
       <c r="U19" s="34"/>
       <c r="V19" s="128"/>
-      <c r="W19" s="877"/>
+      <c r="W19" s="871"/>
       <c r="X19" s="541"/>
       <c r="Y19" s="233"/>
     </row>
@@ -31500,7 +31459,7 @@
       <c r="S20" s="147"/>
       <c r="U20" s="34"/>
       <c r="V20" s="128"/>
-      <c r="W20" s="877"/>
+      <c r="W20" s="871"/>
       <c r="X20" s="34"/>
       <c r="Y20" s="233"/>
     </row>
@@ -31555,8 +31514,8 @@
       <c r="S21" s="147"/>
       <c r="U21" s="34"/>
       <c r="V21" s="128"/>
-      <c r="W21" s="781"/>
-      <c r="X21" s="781"/>
+      <c r="W21" s="797"/>
+      <c r="X21" s="797"/>
       <c r="Y21" s="233"/>
       <c r="Z21" s="128"/>
     </row>
@@ -31667,8 +31626,8 @@
       <c r="S23" s="147"/>
       <c r="U23" s="34"/>
       <c r="V23" s="128"/>
-      <c r="W23" s="782"/>
-      <c r="X23" s="782"/>
+      <c r="W23" s="798"/>
+      <c r="X23" s="798"/>
       <c r="Y23" s="233"/>
       <c r="Z23" s="128"/>
     </row>
@@ -31729,8 +31688,8 @@
       <c r="S24" s="147"/>
       <c r="U24" s="34"/>
       <c r="V24" s="128"/>
-      <c r="W24" s="782"/>
-      <c r="X24" s="782"/>
+      <c r="W24" s="798"/>
+      <c r="X24" s="798"/>
       <c r="Y24" s="233"/>
       <c r="Z24" s="128"/>
     </row>
@@ -31783,8 +31742,8 @@
       </c>
       <c r="U25" s="34"/>
       <c r="V25" s="128"/>
-      <c r="W25" s="783"/>
-      <c r="X25" s="783"/>
+      <c r="W25" s="799"/>
+      <c r="X25" s="799"/>
       <c r="Y25" s="233"/>
       <c r="Z25" s="128"/>
     </row>
@@ -31839,8 +31798,8 @@
       <c r="T26" s="128"/>
       <c r="U26" s="34"/>
       <c r="V26" s="128"/>
-      <c r="W26" s="783"/>
-      <c r="X26" s="783"/>
+      <c r="W26" s="799"/>
+      <c r="X26" s="799"/>
       <c r="Y26" s="233"/>
       <c r="Z26" s="128"/>
     </row>
@@ -31895,9 +31854,9 @@
       <c r="T27" s="128"/>
       <c r="U27" s="34"/>
       <c r="V27" s="128"/>
-      <c r="W27" s="776"/>
-      <c r="X27" s="777"/>
-      <c r="Y27" s="778"/>
+      <c r="W27" s="792"/>
+      <c r="X27" s="793"/>
+      <c r="Y27" s="794"/>
       <c r="Z27" s="128"/>
     </row>
     <row r="28" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -31951,9 +31910,9 @@
       <c r="T28" s="128"/>
       <c r="U28" s="34"/>
       <c r="V28" s="128"/>
-      <c r="W28" s="777"/>
-      <c r="X28" s="777"/>
-      <c r="Y28" s="778"/>
+      <c r="W28" s="793"/>
+      <c r="X28" s="793"/>
+      <c r="Y28" s="794"/>
       <c r="Z28" s="128"/>
     </row>
     <row r="29" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -32544,11 +32503,11 @@
       <c r="J41" s="56"/>
       <c r="K41" s="38"/>
       <c r="L41" s="39"/>
-      <c r="M41" s="794">
+      <c r="M41" s="783">
         <f>SUM(M5:M40)</f>
         <v>1509924.1</v>
       </c>
-      <c r="N41" s="794">
+      <c r="N41" s="783">
         <f>SUM(N5:N40)</f>
         <v>1012291</v>
       </c>
@@ -32580,8 +32539,8 @@
       <c r="L42" s="637">
         <v>3095.88</v>
       </c>
-      <c r="M42" s="795"/>
-      <c r="N42" s="795"/>
+      <c r="M42" s="784"/>
+      <c r="N42" s="784"/>
       <c r="P42" s="34"/>
       <c r="Q42" s="849"/>
     </row>
@@ -33072,26 +33031,26 @@
       <c r="A63" s="98"/>
       <c r="B63" s="99"/>
       <c r="C63" s="1"/>
-      <c r="H63" s="749" t="s">
+      <c r="H63" s="760" t="s">
         <v>11</v>
       </c>
-      <c r="I63" s="750"/>
+      <c r="I63" s="761"/>
       <c r="J63" s="559"/>
-      <c r="K63" s="873">
+      <c r="K63" s="876">
         <f>I61+L61</f>
         <v>340912.75</v>
       </c>
-      <c r="L63" s="874"/>
+      <c r="L63" s="877"/>
       <c r="M63" s="272"/>
       <c r="N63" s="272"/>
       <c r="P63" s="34"/>
       <c r="Q63" s="13"/>
     </row>
     <row r="64" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D64" s="755" t="s">
+      <c r="D64" s="766" t="s">
         <v>12</v>
       </c>
-      <c r="E64" s="755"/>
+      <c r="E64" s="766"/>
       <c r="F64" s="312">
         <f>F61-K63-C61</f>
         <v>1458827.53</v>
@@ -33100,22 +33059,22 @@
       <c r="J64" s="560"/>
     </row>
     <row r="65" spans="2:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D65" s="785" t="s">
+      <c r="D65" s="790" t="s">
         <v>95</v>
       </c>
-      <c r="E65" s="785"/>
+      <c r="E65" s="790"/>
       <c r="F65" s="111">
         <v>-1572197.3</v>
       </c>
-      <c r="I65" s="756" t="s">
+      <c r="I65" s="767" t="s">
         <v>13</v>
       </c>
-      <c r="J65" s="757"/>
-      <c r="K65" s="758">
+      <c r="J65" s="768"/>
+      <c r="K65" s="769">
         <f>F67+F68+F69</f>
         <v>2392765.5300000003</v>
       </c>
-      <c r="L65" s="758"/>
+      <c r="L65" s="769"/>
       <c r="M65" s="404"/>
       <c r="N65" s="404"/>
       <c r="O65" s="579"/>
@@ -33156,11 +33115,11 @@
         <v>15</v>
       </c>
       <c r="J67" s="109"/>
-      <c r="K67" s="875">
+      <c r="K67" s="872">
         <f>-C4</f>
         <v>-2112071.92</v>
       </c>
-      <c r="L67" s="758"/>
+      <c r="L67" s="769"/>
     </row>
     <row r="68" spans="2:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D68" s="110" t="s">
@@ -33177,22 +33136,22 @@
       <c r="C69" s="112">
         <v>44710</v>
       </c>
-      <c r="D69" s="738" t="s">
+      <c r="D69" s="749" t="s">
         <v>18</v>
       </c>
-      <c r="E69" s="739"/>
+      <c r="E69" s="750"/>
       <c r="F69" s="113">
         <v>2546982.16</v>
       </c>
-      <c r="I69" s="870" t="s">
+      <c r="I69" s="873" t="s">
         <v>198</v>
       </c>
-      <c r="J69" s="871"/>
-      <c r="K69" s="872">
+      <c r="J69" s="874"/>
+      <c r="K69" s="875">
         <f>K65+K67</f>
         <v>280693.61000000034</v>
       </c>
-      <c r="L69" s="872"/>
+      <c r="L69" s="875"/>
     </row>
     <row r="70" spans="2:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C70" s="114"/>
@@ -33339,6 +33298,21 @@
     <sortCondition ref="J42:J56"/>
   </sortState>
   <mergeCells count="30">
+    <mergeCell ref="D69:E69"/>
+    <mergeCell ref="I69:J69"/>
+    <mergeCell ref="K69:L69"/>
+    <mergeCell ref="H63:I63"/>
+    <mergeCell ref="K63:L63"/>
+    <mergeCell ref="D64:E64"/>
+    <mergeCell ref="D65:E65"/>
+    <mergeCell ref="I65:J65"/>
+    <mergeCell ref="K65:L65"/>
+    <mergeCell ref="Y27:Y28"/>
+    <mergeCell ref="M41:M42"/>
+    <mergeCell ref="N41:N42"/>
+    <mergeCell ref="Q41:Q42"/>
+    <mergeCell ref="K67:L67"/>
+    <mergeCell ref="M45:N45"/>
     <mergeCell ref="W26:X26"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="W27:X28"/>
@@ -33354,21 +33328,6 @@
     <mergeCell ref="W21:X21"/>
     <mergeCell ref="W23:X24"/>
     <mergeCell ref="W25:X25"/>
-    <mergeCell ref="Y27:Y28"/>
-    <mergeCell ref="M41:M42"/>
-    <mergeCell ref="N41:N42"/>
-    <mergeCell ref="Q41:Q42"/>
-    <mergeCell ref="K67:L67"/>
-    <mergeCell ref="M45:N45"/>
-    <mergeCell ref="D69:E69"/>
-    <mergeCell ref="I69:J69"/>
-    <mergeCell ref="K69:L69"/>
-    <mergeCell ref="H63:I63"/>
-    <mergeCell ref="K63:L63"/>
-    <mergeCell ref="D64:E64"/>
-    <mergeCell ref="D65:E65"/>
-    <mergeCell ref="I65:J65"/>
-    <mergeCell ref="K65:L65"/>
   </mergeCells>
   <pageMargins left="0.28000000000000003" right="0.19" top="0.33" bottom="0.33" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -35943,7 +35902,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="762"/>
+      <c r="B1" s="738"/>
       <c r="C1" s="804" t="s">
         <v>884</v>
       </c>
@@ -35959,7 +35918,7 @@
       <c r="M1" s="805"/>
     </row>
     <row r="2" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="763"/>
+      <c r="B2" s="739"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -35969,21 +35928,21 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:18" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="766" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="767"/>
+      <c r="B3" s="742" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="743"/>
       <c r="D3" s="10"/>
       <c r="E3" s="553"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="768" t="s">
+      <c r="H3" s="744" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="768"/>
+      <c r="I3" s="744"/>
       <c r="K3" s="165"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
-      <c r="P3" s="792" t="s">
+      <c r="P3" s="781" t="s">
         <v>6</v>
       </c>
       <c r="R3" s="802" t="s">
@@ -36001,14 +35960,14 @@
       <c r="D4" s="18">
         <v>44710</v>
       </c>
-      <c r="E4" s="769" t="s">
+      <c r="E4" s="745" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="770"/>
-      <c r="H4" s="771" t="s">
+      <c r="F4" s="746"/>
+      <c r="H4" s="747" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="772"/>
+      <c r="I4" s="748"/>
       <c r="J4" s="556"/>
       <c r="K4" s="562"/>
       <c r="L4" s="563"/>
@@ -36018,7 +35977,7 @@
       <c r="N4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="793"/>
+      <c r="P4" s="782"/>
       <c r="Q4" s="322" t="s">
         <v>217</v>
       </c>
@@ -37790,11 +37749,11 @@
       <c r="L41" s="39">
         <v>18992.37</v>
       </c>
-      <c r="M41" s="794">
+      <c r="M41" s="783">
         <f>SUM(M5:M40)</f>
         <v>1737024</v>
       </c>
-      <c r="N41" s="794">
+      <c r="N41" s="783">
         <f>SUM(N5:N40)</f>
         <v>1314313</v>
       </c>
@@ -37832,8 +37791,8 @@
       <c r="L42" s="52">
         <v>17035.3</v>
       </c>
-      <c r="M42" s="795"/>
-      <c r="N42" s="795"/>
+      <c r="M42" s="784"/>
+      <c r="N42" s="784"/>
       <c r="P42" s="34"/>
       <c r="Q42" s="849"/>
     </row>
@@ -38512,26 +38471,26 @@
       <c r="A69" s="98"/>
       <c r="B69" s="99"/>
       <c r="C69" s="1"/>
-      <c r="H69" s="749" t="s">
+      <c r="H69" s="760" t="s">
         <v>11</v>
       </c>
-      <c r="I69" s="750"/>
+      <c r="I69" s="761"/>
       <c r="J69" s="559"/>
-      <c r="K69" s="873">
+      <c r="K69" s="876">
         <f>I67+L67</f>
         <v>534683.29</v>
       </c>
-      <c r="L69" s="874"/>
+      <c r="L69" s="877"/>
       <c r="M69" s="272"/>
       <c r="N69" s="272"/>
       <c r="P69" s="34"/>
       <c r="Q69" s="13"/>
     </row>
     <row r="70" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D70" s="755" t="s">
+      <c r="D70" s="766" t="s">
         <v>12</v>
       </c>
-      <c r="E70" s="755"/>
+      <c r="E70" s="766"/>
       <c r="F70" s="312">
         <f>F67-K69-C67</f>
         <v>1883028.8699999999</v>
@@ -38540,22 +38499,22 @@
       <c r="J70" s="560"/>
     </row>
     <row r="71" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D71" s="785" t="s">
+      <c r="D71" s="790" t="s">
         <v>95</v>
       </c>
-      <c r="E71" s="785"/>
+      <c r="E71" s="790"/>
       <c r="F71" s="111">
         <v>-2122394.9</v>
       </c>
-      <c r="I71" s="756" t="s">
+      <c r="I71" s="767" t="s">
         <v>13</v>
       </c>
-      <c r="J71" s="757"/>
-      <c r="K71" s="758">
+      <c r="J71" s="768"/>
+      <c r="K71" s="769">
         <f>F73+F74+F75</f>
         <v>2367293.46</v>
       </c>
-      <c r="L71" s="758"/>
+      <c r="L71" s="769"/>
       <c r="M71" s="404"/>
       <c r="N71" s="404"/>
       <c r="O71" s="654"/>
@@ -38596,11 +38555,11 @@
         <v>15</v>
       </c>
       <c r="J73" s="109"/>
-      <c r="K73" s="875">
+      <c r="K73" s="872">
         <f>-C4</f>
         <v>-2546982.16</v>
       </c>
-      <c r="L73" s="758"/>
+      <c r="L73" s="769"/>
     </row>
     <row r="74" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D74" s="110" t="s">
@@ -38617,22 +38576,22 @@
       <c r="C75" s="112">
         <v>44745</v>
       </c>
-      <c r="D75" s="738" t="s">
+      <c r="D75" s="749" t="s">
         <v>18</v>
       </c>
-      <c r="E75" s="739"/>
+      <c r="E75" s="750"/>
       <c r="F75" s="113">
         <v>2355426.54</v>
       </c>
-      <c r="I75" s="740" t="s">
+      <c r="I75" s="751" t="s">
         <v>97</v>
       </c>
-      <c r="J75" s="741"/>
-      <c r="K75" s="742">
+      <c r="J75" s="752"/>
+      <c r="K75" s="753">
         <f>K71+K73</f>
         <v>-179688.70000000019</v>
       </c>
-      <c r="L75" s="742"/>
+      <c r="L75" s="753"/>
     </row>
     <row r="76" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C76" s="114"/>
@@ -38779,17 +38738,6 @@
     <sortCondition ref="B42:B51"/>
   </sortState>
   <mergeCells count="22">
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="R3:R4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="M41:M42"/>
-    <mergeCell ref="N41:N42"/>
-    <mergeCell ref="Q41:Q42"/>
     <mergeCell ref="K73:L73"/>
     <mergeCell ref="D75:E75"/>
     <mergeCell ref="I75:J75"/>
@@ -38801,6 +38749,17 @@
     <mergeCell ref="D71:E71"/>
     <mergeCell ref="I71:J71"/>
     <mergeCell ref="K71:L71"/>
+    <mergeCell ref="R3:R4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="M41:M42"/>
+    <mergeCell ref="N41:N42"/>
+    <mergeCell ref="Q41:Q42"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="P3:P4"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.31496062992125984" bottom="0.39370078740157483" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="5" scale="70" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -38816,8 +38775,8 @@
   </sheetPr>
   <dimension ref="A1:M123"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="B83" sqref="B83"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="E45" sqref="E44:E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -40150,7 +40109,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:13" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:13" ht="32.25" x14ac:dyDescent="0.3">
       <c r="A34" s="454">
         <v>44739</v>
       </c>
@@ -40160,15 +40119,16 @@
       <c r="C34" s="111">
         <v>49528.800000000003</v>
       </c>
-      <c r="D34" s="718">
-        <v>44769</v>
+      <c r="D34" s="884" t="s">
+        <v>1184</v>
       </c>
       <c r="E34" s="717">
-        <v>24074.75</v>
+        <f>24074.75+25454.05</f>
+        <v>49528.800000000003</v>
       </c>
       <c r="F34" s="544">
         <f t="shared" si="0"/>
-        <v>25454.050000000003</v>
+        <v>0</v>
       </c>
       <c r="H34" s="672" t="s">
         <v>1014</v>
@@ -40200,11 +40160,15 @@
       <c r="C35" s="111">
         <v>9215.3700000000008</v>
       </c>
-      <c r="D35" s="412"/>
-      <c r="E35" s="111"/>
+      <c r="D35" s="885">
+        <v>44799</v>
+      </c>
+      <c r="E35" s="886">
+        <v>9215.3700000000008</v>
+      </c>
       <c r="F35" s="544">
         <f t="shared" si="0"/>
-        <v>9215.3700000000008</v>
+        <v>0</v>
       </c>
       <c r="H35" s="675" t="s">
         <v>1015</v>
@@ -40236,11 +40200,15 @@
       <c r="C36" s="111">
         <v>96875.6</v>
       </c>
-      <c r="D36" s="412"/>
-      <c r="E36" s="111"/>
+      <c r="D36" s="885">
+        <v>44799</v>
+      </c>
+      <c r="E36" s="886">
+        <v>96875.6</v>
+      </c>
       <c r="F36" s="544">
         <f t="shared" si="0"/>
-        <v>96875.6</v>
+        <v>0</v>
       </c>
       <c r="H36" s="675" t="s">
         <v>1016</v>
@@ -40272,11 +40240,15 @@
       <c r="C37" s="111">
         <v>26574.6</v>
       </c>
-      <c r="D37" s="412"/>
-      <c r="E37" s="111"/>
+      <c r="D37" s="885">
+        <v>44799</v>
+      </c>
+      <c r="E37" s="886">
+        <v>26574.6</v>
+      </c>
       <c r="F37" s="544">
         <f t="shared" si="0"/>
-        <v>26574.6</v>
+        <v>0</v>
       </c>
       <c r="H37" s="672" t="s">
         <v>1017</v>
@@ -40308,11 +40280,15 @@
       <c r="C38" s="111">
         <v>110618.06</v>
       </c>
-      <c r="D38" s="412"/>
-      <c r="E38" s="111"/>
+      <c r="D38" s="885">
+        <v>44799</v>
+      </c>
+      <c r="E38" s="886">
+        <v>110618.06</v>
+      </c>
       <c r="F38" s="544">
         <f t="shared" si="0"/>
-        <v>110618.06</v>
+        <v>0</v>
       </c>
       <c r="H38" s="675" t="s">
         <v>1018</v>
@@ -40344,11 +40320,15 @@
       <c r="C39" s="111">
         <v>3223.2</v>
       </c>
-      <c r="D39" s="253"/>
-      <c r="E39" s="69"/>
+      <c r="D39" s="885">
+        <v>44799</v>
+      </c>
+      <c r="E39" s="886">
+        <v>3223.2</v>
+      </c>
       <c r="F39" s="111">
         <f t="shared" si="0"/>
-        <v>3223.2</v>
+        <v>0</v>
       </c>
       <c r="H39" s="134"/>
       <c r="I39" s="139"/>
@@ -40370,11 +40350,15 @@
       <c r="C40" s="111">
         <v>65436.19</v>
       </c>
-      <c r="D40" s="253"/>
-      <c r="E40" s="69"/>
+      <c r="D40" s="885">
+        <v>44799</v>
+      </c>
+      <c r="E40" s="886">
+        <v>65436.19</v>
+      </c>
       <c r="F40" s="111">
         <f t="shared" si="0"/>
-        <v>65436.19</v>
+        <v>0</v>
       </c>
       <c r="H40" s="134"/>
       <c r="I40" s="139"/>
@@ -40396,11 +40380,15 @@
       <c r="C41" s="111">
         <v>60853.03</v>
       </c>
-      <c r="D41" s="253"/>
-      <c r="E41" s="69"/>
+      <c r="D41" s="885">
+        <v>44799</v>
+      </c>
+      <c r="E41" s="886">
+        <v>60853.03</v>
+      </c>
       <c r="F41" s="111">
         <f t="shared" si="0"/>
-        <v>60853.03</v>
+        <v>0</v>
       </c>
       <c r="H41" s="134"/>
       <c r="I41" s="139"/>
@@ -40422,11 +40410,15 @@
       <c r="C42" s="111">
         <v>5205</v>
       </c>
-      <c r="D42" s="253"/>
-      <c r="E42" s="69"/>
+      <c r="D42" s="885">
+        <v>44799</v>
+      </c>
+      <c r="E42" s="886">
+        <v>5205</v>
+      </c>
       <c r="F42" s="111">
         <f t="shared" si="0"/>
-        <v>5205</v>
+        <v>0</v>
       </c>
       <c r="H42" s="134"/>
       <c r="I42" s="139"/>
@@ -40929,11 +40921,11 @@
       <c r="D67" s="407"/>
       <c r="E67" s="395">
         <f>SUM(E3:E66)</f>
-        <v>1718939.8</v>
+        <v>2122394.9000000004</v>
       </c>
       <c r="F67" s="153">
         <f>SUM(F3:F66)</f>
-        <v>403455.10000000009</v>
+        <v>0</v>
       </c>
       <c r="H67" s="838" t="s">
         <v>594</v>
@@ -44414,7 +44406,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="762"/>
+      <c r="B1" s="738"/>
       <c r="C1" s="804" t="s">
         <v>1027</v>
       </c>
@@ -44430,7 +44422,7 @@
       <c r="M1" s="805"/>
     </row>
     <row r="2" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="763"/>
+      <c r="B2" s="739"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -44440,21 +44432,21 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:18" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="766" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="767"/>
+      <c r="B3" s="742" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="743"/>
       <c r="D3" s="10"/>
       <c r="E3" s="553"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="768" t="s">
+      <c r="H3" s="744" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="768"/>
+      <c r="I3" s="744"/>
       <c r="K3" s="165"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
-      <c r="P3" s="792" t="s">
+      <c r="P3" s="781" t="s">
         <v>6</v>
       </c>
       <c r="R3" s="802" t="s">
@@ -44472,14 +44464,14 @@
       <c r="D4" s="18">
         <v>44745</v>
       </c>
-      <c r="E4" s="769" t="s">
+      <c r="E4" s="745" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="770"/>
-      <c r="H4" s="771" t="s">
+      <c r="F4" s="746"/>
+      <c r="H4" s="747" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="772"/>
+      <c r="I4" s="748"/>
       <c r="J4" s="556"/>
       <c r="K4" s="562"/>
       <c r="L4" s="563"/>
@@ -44489,7 +44481,7 @@
       <c r="N4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="793"/>
+      <c r="P4" s="782"/>
       <c r="Q4" s="322" t="s">
         <v>217</v>
       </c>
@@ -46227,11 +46219,11 @@
       <c r="L41" s="39">
         <v>3442.5</v>
       </c>
-      <c r="M41" s="794">
+      <c r="M41" s="783">
         <f>SUM(M5:M40)</f>
         <v>2180659.5</v>
       </c>
-      <c r="N41" s="794">
+      <c r="N41" s="783">
         <f>SUM(N5:N40)</f>
         <v>1072718</v>
       </c>
@@ -46269,8 +46261,8 @@
       <c r="L42" s="702">
         <v>28000</v>
       </c>
-      <c r="M42" s="795"/>
-      <c r="N42" s="795"/>
+      <c r="M42" s="784"/>
+      <c r="N42" s="784"/>
       <c r="P42" s="34"/>
       <c r="Q42" s="849"/>
     </row>
@@ -46874,26 +46866,26 @@
       <c r="A69" s="98"/>
       <c r="B69" s="99"/>
       <c r="C69" s="1"/>
-      <c r="H69" s="749" t="s">
+      <c r="H69" s="760" t="s">
         <v>11</v>
       </c>
-      <c r="I69" s="750"/>
+      <c r="I69" s="761"/>
       <c r="J69" s="559"/>
-      <c r="K69" s="873">
+      <c r="K69" s="876">
         <f>I67+L67</f>
         <v>515778.65000000026</v>
       </c>
-      <c r="L69" s="874"/>
+      <c r="L69" s="877"/>
       <c r="M69" s="272"/>
       <c r="N69" s="272"/>
       <c r="P69" s="34"/>
       <c r="Q69" s="13"/>
     </row>
     <row r="70" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D70" s="755" t="s">
+      <c r="D70" s="766" t="s">
         <v>12</v>
       </c>
-      <c r="E70" s="755"/>
+      <c r="E70" s="766"/>
       <c r="F70" s="312">
         <f>F67-K69-C67</f>
         <v>1573910.5599999998</v>
@@ -46902,22 +46894,22 @@
       <c r="J70" s="560"/>
     </row>
     <row r="71" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D71" s="785" t="s">
+      <c r="D71" s="790" t="s">
         <v>95</v>
       </c>
-      <c r="E71" s="785"/>
+      <c r="E71" s="790"/>
       <c r="F71" s="111">
         <v>-1727771.26</v>
       </c>
-      <c r="I71" s="756" t="s">
+      <c r="I71" s="767" t="s">
         <v>13</v>
       </c>
-      <c r="J71" s="757"/>
-      <c r="K71" s="758">
+      <c r="J71" s="768"/>
+      <c r="K71" s="769">
         <f>F73+F74+F75</f>
         <v>2141254.8899999997</v>
       </c>
-      <c r="L71" s="758"/>
+      <c r="L71" s="769"/>
       <c r="M71" s="404"/>
       <c r="N71" s="404"/>
       <c r="O71" s="654"/>
@@ -46958,11 +46950,11 @@
         <v>15</v>
       </c>
       <c r="J73" s="109"/>
-      <c r="K73" s="875">
+      <c r="K73" s="872">
         <f>-C4</f>
         <v>-2355426.54</v>
       </c>
-      <c r="L73" s="758"/>
+      <c r="L73" s="769"/>
     </row>
     <row r="74" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D74" s="110" t="s">
@@ -46979,22 +46971,22 @@
       <c r="C75" s="112">
         <v>44773</v>
       </c>
-      <c r="D75" s="738" t="s">
+      <c r="D75" s="749" t="s">
         <v>18</v>
       </c>
-      <c r="E75" s="739"/>
+      <c r="E75" s="750"/>
       <c r="F75" s="113">
         <v>2274653.09</v>
       </c>
-      <c r="I75" s="870" t="s">
+      <c r="I75" s="873" t="s">
         <v>97</v>
       </c>
-      <c r="J75" s="871"/>
-      <c r="K75" s="872">
+      <c r="J75" s="874"/>
+      <c r="K75" s="875">
         <f>K71+K73</f>
         <v>-214171.65000000037</v>
       </c>
-      <c r="L75" s="872"/>
+      <c r="L75" s="875"/>
     </row>
     <row r="76" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C76" s="114"/>
@@ -47141,6 +47133,12 @@
     <sortCondition ref="B35:B44"/>
   </sortState>
   <mergeCells count="22">
+    <mergeCell ref="M45:N45"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="H4:I4"/>
@@ -47157,12 +47155,6 @@
     <mergeCell ref="H69:I69"/>
     <mergeCell ref="K69:L69"/>
     <mergeCell ref="Q41:Q42"/>
-    <mergeCell ref="M45:N45"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.19685039370078741" top="0.31496062992125984" bottom="0.19685039370078741" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="5" scale="70" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -47178,8 +47170,8 @@
   </sheetPr>
   <dimension ref="A1:M123"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39:E39"/>
+    <sheetView topLeftCell="D16" workbookViewId="0">
+      <selection activeCell="O40" sqref="O40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -47269,11 +47261,15 @@
       <c r="C3" s="111">
         <v>67911.399999999994</v>
       </c>
-      <c r="D3" s="412"/>
-      <c r="E3" s="111"/>
+      <c r="D3" s="885">
+        <v>44799</v>
+      </c>
+      <c r="E3" s="886">
+        <v>67911.399999999994</v>
+      </c>
       <c r="F3" s="410">
         <f>C3-E3</f>
-        <v>67911.399999999994</v>
+        <v>0</v>
       </c>
       <c r="H3" s="704" t="s">
         <v>1119</v>
@@ -47305,11 +47301,15 @@
       <c r="C4" s="111">
         <v>73363.8</v>
       </c>
-      <c r="D4" s="412"/>
-      <c r="E4" s="111"/>
+      <c r="D4" s="885">
+        <v>44799</v>
+      </c>
+      <c r="E4" s="886">
+        <v>73363.8</v>
+      </c>
       <c r="F4" s="544">
         <f t="shared" ref="F4:F65" si="0">C4-E4</f>
-        <v>73363.8</v>
+        <v>0</v>
       </c>
       <c r="G4" s="138"/>
       <c r="H4" s="704" t="s">
@@ -47342,11 +47342,15 @@
       <c r="C5" s="111">
         <v>31164.35</v>
       </c>
-      <c r="D5" s="412"/>
-      <c r="E5" s="111"/>
+      <c r="D5" s="885">
+        <v>44799</v>
+      </c>
+      <c r="E5" s="886">
+        <v>31164.35</v>
+      </c>
       <c r="F5" s="544">
         <f t="shared" si="0"/>
-        <v>31164.35</v>
+        <v>0</v>
       </c>
       <c r="H5" s="704" t="s">
         <v>1121</v>
@@ -47378,11 +47382,15 @@
       <c r="C6" s="111">
         <v>58616</v>
       </c>
-      <c r="D6" s="412"/>
-      <c r="E6" s="111"/>
+      <c r="D6" s="885">
+        <v>44799</v>
+      </c>
+      <c r="E6" s="886">
+        <v>58616</v>
+      </c>
       <c r="F6" s="544">
         <f t="shared" si="0"/>
-        <v>58616</v>
+        <v>0</v>
       </c>
       <c r="H6" s="704" t="s">
         <v>1122</v>
@@ -47414,11 +47422,15 @@
       <c r="C7" s="111">
         <v>106705.96</v>
       </c>
-      <c r="D7" s="412"/>
-      <c r="E7" s="111"/>
+      <c r="D7" s="885">
+        <v>44799</v>
+      </c>
+      <c r="E7" s="886">
+        <v>106705.96</v>
+      </c>
       <c r="F7" s="544">
         <f t="shared" si="0"/>
-        <v>106705.96</v>
+        <v>0</v>
       </c>
       <c r="H7" s="704" t="s">
         <v>1123</v>
@@ -47450,11 +47462,15 @@
       <c r="C8" s="111">
         <v>68357.89</v>
       </c>
-      <c r="D8" s="412"/>
-      <c r="E8" s="111"/>
+      <c r="D8" s="885">
+        <v>44799</v>
+      </c>
+      <c r="E8" s="886">
+        <v>68357.89</v>
+      </c>
       <c r="F8" s="544">
         <f t="shared" si="0"/>
-        <v>68357.89</v>
+        <v>0</v>
       </c>
       <c r="H8" s="704" t="s">
         <v>1124</v>
@@ -47486,11 +47502,15 @@
       <c r="C9" s="111">
         <v>39927.050000000003</v>
       </c>
-      <c r="D9" s="412"/>
-      <c r="E9" s="111"/>
+      <c r="D9" s="885">
+        <v>44799</v>
+      </c>
+      <c r="E9" s="886">
+        <v>39927.050000000003</v>
+      </c>
       <c r="F9" s="544">
         <f t="shared" si="0"/>
-        <v>39927.050000000003</v>
+        <v>0</v>
       </c>
       <c r="H9" s="704" t="s">
         <v>1124</v>
@@ -47522,11 +47542,15 @@
       <c r="C10" s="111">
         <v>121513</v>
       </c>
-      <c r="D10" s="412"/>
-      <c r="E10" s="111"/>
+      <c r="D10" s="885">
+        <v>44799</v>
+      </c>
+      <c r="E10" s="886">
+        <v>121513</v>
+      </c>
       <c r="F10" s="544">
         <f t="shared" si="0"/>
-        <v>121513</v>
+        <v>0</v>
       </c>
       <c r="G10" s="138"/>
       <c r="H10" s="704" t="s">
@@ -47559,11 +47583,15 @@
       <c r="C11" s="111">
         <v>60297.8</v>
       </c>
-      <c r="D11" s="412"/>
-      <c r="E11" s="111"/>
+      <c r="D11" s="885">
+        <v>44799</v>
+      </c>
+      <c r="E11" s="886">
+        <v>60297.8</v>
+      </c>
       <c r="F11" s="544">
         <f t="shared" si="0"/>
-        <v>60297.8</v>
+        <v>0</v>
       </c>
       <c r="H11" s="704" t="s">
         <v>1125</v>
@@ -47595,11 +47623,15 @@
       <c r="C12" s="111">
         <v>105453.7</v>
       </c>
-      <c r="D12" s="412"/>
-      <c r="E12" s="111"/>
+      <c r="D12" s="885">
+        <v>44799</v>
+      </c>
+      <c r="E12" s="886">
+        <v>105453.7</v>
+      </c>
       <c r="F12" s="544">
         <f t="shared" si="0"/>
-        <v>105453.7</v>
+        <v>0</v>
       </c>
       <c r="H12" s="704" t="s">
         <v>1126</v>
@@ -47631,11 +47663,15 @@
       <c r="C13" s="111">
         <v>65012.85</v>
       </c>
-      <c r="D13" s="412"/>
-      <c r="E13" s="111"/>
+      <c r="D13" s="885">
+        <v>44799</v>
+      </c>
+      <c r="E13" s="886">
+        <v>65012.85</v>
+      </c>
       <c r="F13" s="544">
         <f t="shared" si="0"/>
-        <v>65012.85</v>
+        <v>0</v>
       </c>
       <c r="H13" s="704" t="s">
         <v>1127</v>
@@ -47667,11 +47703,15 @@
       <c r="C14" s="111">
         <v>83843.7</v>
       </c>
-      <c r="D14" s="412"/>
-      <c r="E14" s="111"/>
+      <c r="D14" s="885">
+        <v>44799</v>
+      </c>
+      <c r="E14" s="886">
+        <v>83843.7</v>
+      </c>
       <c r="F14" s="544">
         <f t="shared" si="0"/>
-        <v>83843.7</v>
+        <v>0</v>
       </c>
       <c r="H14" s="704" t="s">
         <v>1128</v>
@@ -47703,11 +47743,15 @@
       <c r="C15" s="111">
         <v>11248</v>
       </c>
-      <c r="D15" s="412"/>
-      <c r="E15" s="111"/>
+      <c r="D15" s="885">
+        <v>44799</v>
+      </c>
+      <c r="E15" s="886">
+        <v>11248</v>
+      </c>
       <c r="F15" s="544">
         <f t="shared" si="0"/>
-        <v>11248</v>
+        <v>0</v>
       </c>
       <c r="H15" s="704" t="s">
         <v>1128</v>
@@ -47739,11 +47783,15 @@
       <c r="C16" s="111">
         <v>30498.9</v>
       </c>
-      <c r="D16" s="412"/>
-      <c r="E16" s="111"/>
+      <c r="D16" s="885">
+        <v>44799</v>
+      </c>
+      <c r="E16" s="886">
+        <v>30498.9</v>
+      </c>
       <c r="F16" s="544">
         <f t="shared" si="0"/>
-        <v>30498.9</v>
+        <v>0</v>
       </c>
       <c r="H16" s="704" t="s">
         <v>1129</v>
@@ -47775,11 +47823,15 @@
       <c r="C17" s="111">
         <v>4920</v>
       </c>
-      <c r="D17" s="412"/>
-      <c r="E17" s="111"/>
+      <c r="D17" s="885">
+        <v>44799</v>
+      </c>
+      <c r="E17" s="886">
+        <v>4920</v>
+      </c>
       <c r="F17" s="544">
         <f t="shared" si="0"/>
-        <v>4920</v>
+        <v>0</v>
       </c>
       <c r="H17" s="704" t="s">
         <v>1130</v>
@@ -47811,11 +47863,15 @@
       <c r="C18" s="111">
         <v>97808.75</v>
       </c>
-      <c r="D18" s="412"/>
-      <c r="E18" s="111"/>
+      <c r="D18" s="885">
+        <v>44799</v>
+      </c>
+      <c r="E18" s="886">
+        <v>97808.75</v>
+      </c>
       <c r="F18" s="544">
         <f t="shared" si="0"/>
-        <v>97808.75</v>
+        <v>0</v>
       </c>
       <c r="H18" s="704" t="s">
         <v>1131</v>
@@ -47847,11 +47903,15 @@
       <c r="C19" s="111">
         <v>70509.3</v>
       </c>
-      <c r="D19" s="412"/>
-      <c r="E19" s="111"/>
+      <c r="D19" s="885">
+        <v>44799</v>
+      </c>
+      <c r="E19" s="886">
+        <v>70509.3</v>
+      </c>
       <c r="F19" s="544">
         <f t="shared" si="0"/>
-        <v>70509.3</v>
+        <v>0</v>
       </c>
       <c r="H19" s="704" t="s">
         <v>1132</v>
@@ -47883,11 +47943,15 @@
       <c r="C20" s="111">
         <v>72783.5</v>
       </c>
-      <c r="D20" s="412"/>
-      <c r="E20" s="111"/>
+      <c r="D20" s="885">
+        <v>44799</v>
+      </c>
+      <c r="E20" s="886">
+        <v>72783.5</v>
+      </c>
       <c r="F20" s="544">
         <f t="shared" si="0"/>
-        <v>72783.5</v>
+        <v>0</v>
       </c>
       <c r="H20" s="704" t="s">
         <v>1133</v>
@@ -47919,11 +47983,15 @@
       <c r="C21" s="111">
         <v>40894.36</v>
       </c>
-      <c r="D21" s="412"/>
-      <c r="E21" s="111"/>
+      <c r="D21" s="885">
+        <v>44799</v>
+      </c>
+      <c r="E21" s="886">
+        <v>40894.36</v>
+      </c>
       <c r="F21" s="544">
         <f t="shared" si="0"/>
-        <v>40894.36</v>
+        <v>0</v>
       </c>
       <c r="H21" s="704" t="s">
         <v>1134</v>
@@ -47955,11 +48023,15 @@
       <c r="C22" s="111">
         <v>69612.42</v>
       </c>
-      <c r="D22" s="412"/>
-      <c r="E22" s="111"/>
+      <c r="D22" s="885">
+        <v>44799</v>
+      </c>
+      <c r="E22" s="886">
+        <v>69612.42</v>
+      </c>
       <c r="F22" s="544">
         <f t="shared" si="0"/>
-        <v>69612.42</v>
+        <v>0</v>
       </c>
       <c r="G22" s="644"/>
       <c r="H22" s="704" t="s">
@@ -47992,11 +48064,15 @@
       <c r="C23" s="111">
         <v>111046</v>
       </c>
-      <c r="D23" s="412"/>
-      <c r="E23" s="111"/>
+      <c r="D23" s="885">
+        <v>44799</v>
+      </c>
+      <c r="E23" s="886">
+        <v>111046</v>
+      </c>
       <c r="F23" s="544">
         <f t="shared" si="0"/>
-        <v>111046</v>
+        <v>0</v>
       </c>
       <c r="G23" s="2"/>
       <c r="H23" s="704" t="s">
@@ -48025,11 +48101,15 @@
       <c r="C24" s="583">
         <v>3984</v>
       </c>
-      <c r="D24" s="582"/>
-      <c r="E24" s="583"/>
+      <c r="D24" s="885">
+        <v>44799</v>
+      </c>
+      <c r="E24" s="886">
+        <v>3984</v>
+      </c>
       <c r="F24" s="205">
         <f t="shared" si="0"/>
-        <v>3984</v>
+        <v>0</v>
       </c>
       <c r="G24" s="2"/>
       <c r="H24" s="704" t="s">
@@ -48997,11 +49077,11 @@
       <c r="D67" s="407"/>
       <c r="E67" s="395">
         <f>SUM(E3:E66)</f>
-        <v>0</v>
+        <v>1395472.73</v>
       </c>
       <c r="F67" s="153">
         <f>SUM(F3:F66)</f>
-        <v>1727771.26</v>
+        <v>332298.53000000003</v>
       </c>
       <c r="H67" s="838" t="s">
         <v>594</v>
@@ -49633,8 +49713,8 @@
   </sheetPr>
   <dimension ref="A1:S97"/>
   <sheetViews>
-    <sheetView topLeftCell="I7" workbookViewId="0">
-      <selection activeCell="Q20" sqref="Q20"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -49660,7 +49740,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="762"/>
+      <c r="B1" s="738"/>
       <c r="C1" s="804" t="s">
         <v>1144</v>
       </c>
@@ -49676,7 +49756,7 @@
       <c r="M1" s="805"/>
     </row>
     <row r="2" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="763"/>
+      <c r="B2" s="739"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -49686,21 +49766,21 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:19" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="766" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="767"/>
+      <c r="B3" s="742" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="743"/>
       <c r="D3" s="10"/>
       <c r="E3" s="553"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="768" t="s">
+      <c r="H3" s="744" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="768"/>
+      <c r="I3" s="744"/>
       <c r="K3" s="165"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
-      <c r="P3" s="792" t="s">
+      <c r="P3" s="781" t="s">
         <v>6</v>
       </c>
       <c r="R3" s="802" t="s">
@@ -49718,14 +49798,14 @@
       <c r="D4" s="18">
         <v>44773</v>
       </c>
-      <c r="E4" s="769" t="s">
+      <c r="E4" s="745" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="770"/>
-      <c r="H4" s="771" t="s">
+      <c r="F4" s="746"/>
+      <c r="H4" s="747" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="772"/>
+      <c r="I4" s="748"/>
       <c r="J4" s="556"/>
       <c r="K4" s="562"/>
       <c r="L4" s="563"/>
@@ -49735,7 +49815,7 @@
       <c r="N4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="793"/>
+      <c r="P4" s="782"/>
       <c r="Q4" s="322" t="s">
         <v>217</v>
       </c>
@@ -51265,11 +51345,11 @@
       <c r="L41" s="39">
         <v>15889</v>
       </c>
-      <c r="M41" s="794">
+      <c r="M41" s="783">
         <f>SUM(M5:M40)</f>
         <v>804697.68</v>
       </c>
-      <c r="N41" s="794">
+      <c r="N41" s="783">
         <f>SUM(N5:N40)</f>
         <v>707448</v>
       </c>
@@ -51301,8 +51381,8 @@
       <c r="L42" s="702">
         <v>17693</v>
       </c>
-      <c r="M42" s="795"/>
-      <c r="N42" s="795"/>
+      <c r="M42" s="784"/>
+      <c r="N42" s="784"/>
       <c r="P42" s="34"/>
       <c r="Q42" s="849"/>
     </row>
@@ -51784,26 +51864,26 @@
       <c r="A69" s="98"/>
       <c r="B69" s="99"/>
       <c r="C69" s="1"/>
-      <c r="H69" s="749" t="s">
+      <c r="H69" s="760" t="s">
         <v>11</v>
       </c>
-      <c r="I69" s="750"/>
+      <c r="I69" s="761"/>
       <c r="J69" s="559"/>
-      <c r="K69" s="873">
+      <c r="K69" s="876">
         <f>I67+L67</f>
         <v>110669</v>
       </c>
-      <c r="L69" s="874"/>
+      <c r="L69" s="877"/>
       <c r="M69" s="272"/>
       <c r="N69" s="272"/>
       <c r="P69" s="34"/>
       <c r="Q69" s="13"/>
     </row>
     <row r="70" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D70" s="755" t="s">
+      <c r="D70" s="766" t="s">
         <v>12</v>
       </c>
-      <c r="E70" s="755"/>
+      <c r="E70" s="766"/>
       <c r="F70" s="312">
         <f>F67-K69-C67</f>
         <v>1520767</v>
@@ -51812,22 +51892,22 @@
       <c r="J70" s="560"/>
     </row>
     <row r="71" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D71" s="785" t="s">
+      <c r="D71" s="790" t="s">
         <v>95</v>
       </c>
-      <c r="E71" s="785"/>
+      <c r="E71" s="790"/>
       <c r="F71" s="111">
         <v>0</v>
       </c>
-      <c r="I71" s="756" t="s">
+      <c r="I71" s="767" t="s">
         <v>13</v>
       </c>
-      <c r="J71" s="757"/>
-      <c r="K71" s="758">
+      <c r="J71" s="768"/>
+      <c r="K71" s="769">
         <f>F73+F74+F75</f>
         <v>1520767</v>
       </c>
-      <c r="L71" s="758"/>
+      <c r="L71" s="769"/>
       <c r="M71" s="404"/>
       <c r="N71" s="404"/>
       <c r="O71" s="654"/>
@@ -51868,11 +51948,11 @@
         <v>15</v>
       </c>
       <c r="J73" s="109"/>
-      <c r="K73" s="875">
+      <c r="K73" s="872">
         <f>-C4</f>
         <v>-2274653.09</v>
       </c>
-      <c r="L73" s="758"/>
+      <c r="L73" s="769"/>
     </row>
     <row r="74" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D74" s="110" t="s">
@@ -51887,22 +51967,22 @@
     </row>
     <row r="75" spans="1:17" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C75" s="112"/>
-      <c r="D75" s="738" t="s">
+      <c r="D75" s="749" t="s">
         <v>18</v>
       </c>
-      <c r="E75" s="739"/>
+      <c r="E75" s="750"/>
       <c r="F75" s="113">
         <v>0</v>
       </c>
-      <c r="I75" s="870" t="s">
+      <c r="I75" s="873" t="s">
         <v>97</v>
       </c>
-      <c r="J75" s="871"/>
-      <c r="K75" s="872">
+      <c r="J75" s="874"/>
+      <c r="K75" s="875">
         <f>K71+K73</f>
         <v>-753886.08999999985</v>
       </c>
-      <c r="L75" s="872"/>
+      <c r="L75" s="875"/>
     </row>
     <row r="76" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C76" s="114"/>
@@ -52046,6 +52126,12 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="M45:N45"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="H4:I4"/>
@@ -52062,12 +52148,6 @@
     <mergeCell ref="H69:I69"/>
     <mergeCell ref="K69:L69"/>
     <mergeCell ref="Q41:Q42"/>
-    <mergeCell ref="M45:N45"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="5" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -52083,8 +52163,8 @@
   </sheetPr>
   <dimension ref="A1:M123"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -54212,7 +54292,6 @@
     <mergeCell ref="F68:F69"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -54276,23 +54355,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="762"/>
-      <c r="C1" s="764" t="s">
+      <c r="B1" s="738"/>
+      <c r="C1" s="740" t="s">
         <v>208</v>
       </c>
-      <c r="D1" s="765"/>
-      <c r="E1" s="765"/>
-      <c r="F1" s="765"/>
-      <c r="G1" s="765"/>
-      <c r="H1" s="765"/>
-      <c r="I1" s="765"/>
-      <c r="J1" s="765"/>
-      <c r="K1" s="765"/>
-      <c r="L1" s="765"/>
-      <c r="M1" s="765"/>
+      <c r="D1" s="741"/>
+      <c r="E1" s="741"/>
+      <c r="F1" s="741"/>
+      <c r="G1" s="741"/>
+      <c r="H1" s="741"/>
+      <c r="I1" s="741"/>
+      <c r="J1" s="741"/>
+      <c r="K1" s="741"/>
+      <c r="L1" s="741"/>
+      <c r="M1" s="741"/>
     </row>
     <row r="2" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="763"/>
+      <c r="B2" s="739"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -54302,21 +54381,21 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:25" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="766" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="767"/>
+      <c r="B3" s="742" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="743"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="768" t="s">
+      <c r="H3" s="744" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="768"/>
+      <c r="I3" s="744"/>
       <c r="K3" s="165"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
-      <c r="P3" s="792" t="s">
+      <c r="P3" s="781" t="s">
         <v>6</v>
       </c>
     </row>
@@ -54331,14 +54410,14 @@
       <c r="D4" s="18">
         <v>44507</v>
       </c>
-      <c r="E4" s="769" t="s">
+      <c r="E4" s="745" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="770"/>
-      <c r="H4" s="771" t="s">
+      <c r="F4" s="746"/>
+      <c r="H4" s="747" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="772"/>
+      <c r="I4" s="748"/>
       <c r="J4" s="19"/>
       <c r="K4" s="166"/>
       <c r="L4" s="20"/>
@@ -54348,14 +54427,14 @@
       <c r="N4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="793"/>
+      <c r="P4" s="782"/>
       <c r="Q4" s="286" t="s">
         <v>209</v>
       </c>
-      <c r="W4" s="775" t="s">
+      <c r="W4" s="791" t="s">
         <v>124</v>
       </c>
-      <c r="X4" s="775"/>
+      <c r="X4" s="791"/>
       <c r="Y4" s="227"/>
     </row>
     <row r="5" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -54406,8 +54485,8 @@
         <f>20000+7936</f>
         <v>27936</v>
       </c>
-      <c r="W5" s="775"/>
-      <c r="X5" s="775"/>
+      <c r="W5" s="791"/>
+      <c r="X5" s="791"/>
       <c r="Y5" s="233"/>
     </row>
     <row r="6" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -55178,7 +55257,7 @@
         <v>26370</v>
       </c>
       <c r="S19" s="147"/>
-      <c r="W19" s="779">
+      <c r="W19" s="795">
         <f>SUM(W6:W18)</f>
         <v>935136</v>
       </c>
@@ -55230,7 +55309,7 @@
         <v>16395.830000000002</v>
       </c>
       <c r="S20" s="147"/>
-      <c r="W20" s="780"/>
+      <c r="W20" s="796"/>
       <c r="X20" s="268"/>
       <c r="Y20" s="233"/>
     </row>
@@ -55279,8 +55358,8 @@
         <v>19188.82</v>
       </c>
       <c r="S21" s="147"/>
-      <c r="W21" s="781"/>
-      <c r="X21" s="781"/>
+      <c r="W21" s="797"/>
+      <c r="X21" s="797"/>
       <c r="Y21" s="233"/>
       <c r="Z21" s="128"/>
     </row>
@@ -55381,8 +55460,8 @@
         <v>45217.29</v>
       </c>
       <c r="S23" s="147"/>
-      <c r="W23" s="782"/>
-      <c r="X23" s="782"/>
+      <c r="W23" s="798"/>
+      <c r="X23" s="798"/>
       <c r="Y23" s="233"/>
       <c r="Z23" s="128"/>
     </row>
@@ -55436,8 +55515,8 @@
         <v>23159.17</v>
       </c>
       <c r="S24" s="147"/>
-      <c r="W24" s="782"/>
-      <c r="X24" s="782"/>
+      <c r="W24" s="798"/>
+      <c r="X24" s="798"/>
       <c r="Y24" s="233"/>
       <c r="Z24" s="128"/>
     </row>
@@ -55483,8 +55562,8 @@
       <c r="R25" s="285">
         <v>28952</v>
       </c>
-      <c r="W25" s="783"/>
-      <c r="X25" s="783"/>
+      <c r="W25" s="799"/>
+      <c r="X25" s="799"/>
       <c r="Y25" s="233"/>
       <c r="Z25" s="128"/>
     </row>
@@ -55535,8 +55614,8 @@
       <c r="R26" s="285">
         <v>21771.5</v>
       </c>
-      <c r="W26" s="783"/>
-      <c r="X26" s="783"/>
+      <c r="W26" s="799"/>
+      <c r="X26" s="799"/>
       <c r="Y26" s="233"/>
       <c r="Z26" s="128"/>
     </row>
@@ -55584,9 +55663,9 @@
       <c r="R27" s="285">
         <v>14637</v>
       </c>
-      <c r="W27" s="776"/>
-      <c r="X27" s="777"/>
-      <c r="Y27" s="778"/>
+      <c r="W27" s="792"/>
+      <c r="X27" s="793"/>
+      <c r="Y27" s="794"/>
       <c r="Z27" s="128"/>
     </row>
     <row r="28" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -55636,9 +55715,9 @@
       <c r="R28" s="285">
         <v>0</v>
       </c>
-      <c r="W28" s="777"/>
-      <c r="X28" s="777"/>
-      <c r="Y28" s="778"/>
+      <c r="W28" s="793"/>
+      <c r="X28" s="793"/>
+      <c r="Y28" s="794"/>
       <c r="Z28" s="128"/>
     </row>
     <row r="29" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -55973,11 +56052,11 @@
       <c r="L36" s="44">
         <v>5940</v>
       </c>
-      <c r="M36" s="794">
+      <c r="M36" s="783">
         <f>SUM(M5:M35)</f>
         <v>321168.83</v>
       </c>
-      <c r="N36" s="796">
+      <c r="N36" s="785">
         <f>SUM(N5:N35)</f>
         <v>467016</v>
       </c>
@@ -55985,7 +56064,7 @@
       <c r="P36" s="277">
         <v>0</v>
       </c>
-      <c r="Q36" s="798">
+      <c r="Q36" s="787">
         <f>SUM(Q5:Q35)</f>
         <v>-637069.14000000013</v>
       </c>
@@ -56020,13 +56099,13 @@
       <c r="L37" s="61">
         <v>7929.62</v>
       </c>
-      <c r="M37" s="795"/>
-      <c r="N37" s="797"/>
+      <c r="M37" s="784"/>
+      <c r="N37" s="786"/>
       <c r="O37" s="276"/>
       <c r="P37" s="277">
         <v>0</v>
       </c>
-      <c r="Q37" s="799"/>
+      <c r="Q37" s="788"/>
     </row>
     <row r="38" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="23"/>
@@ -56316,26 +56395,26 @@
       <c r="A52" s="98"/>
       <c r="B52" s="99"/>
       <c r="C52" s="1"/>
-      <c r="H52" s="749" t="s">
+      <c r="H52" s="760" t="s">
         <v>11</v>
       </c>
-      <c r="I52" s="750"/>
+      <c r="I52" s="761"/>
       <c r="J52" s="100"/>
-      <c r="K52" s="751">
+      <c r="K52" s="762">
         <f>I50+L50</f>
         <v>71911.59</v>
       </c>
-      <c r="L52" s="784"/>
+      <c r="L52" s="789"/>
       <c r="M52" s="272"/>
       <c r="N52" s="272"/>
       <c r="P52" s="34"/>
       <c r="Q52" s="13"/>
     </row>
     <row r="53" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D53" s="755" t="s">
+      <c r="D53" s="766" t="s">
         <v>12</v>
       </c>
-      <c r="E53" s="755"/>
+      <c r="E53" s="766"/>
       <c r="F53" s="312">
         <f>F50-K52-C50</f>
         <v>-25952.549999999814</v>
@@ -56344,29 +56423,29 @@
       <c r="J53" s="103"/>
     </row>
     <row r="54" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D54" s="785" t="s">
+      <c r="D54" s="790" t="s">
         <v>95</v>
       </c>
-      <c r="E54" s="785"/>
+      <c r="E54" s="790"/>
       <c r="F54" s="111">
         <v>-706888.38</v>
       </c>
-      <c r="I54" s="756" t="s">
+      <c r="I54" s="767" t="s">
         <v>13</v>
       </c>
-      <c r="J54" s="757"/>
-      <c r="K54" s="758">
+      <c r="J54" s="768"/>
+      <c r="K54" s="769">
         <f>F56+F57+F58</f>
         <v>1308778.3500000003</v>
       </c>
-      <c r="L54" s="758"/>
-      <c r="M54" s="786" t="s">
+      <c r="L54" s="769"/>
+      <c r="M54" s="775" t="s">
         <v>211</v>
       </c>
-      <c r="N54" s="787"/>
-      <c r="O54" s="787"/>
-      <c r="P54" s="787"/>
-      <c r="Q54" s="788"/>
+      <c r="N54" s="776"/>
+      <c r="O54" s="776"/>
+      <c r="P54" s="776"/>
+      <c r="Q54" s="777"/>
     </row>
     <row r="55" spans="1:17" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D55" s="313" t="s">
@@ -56380,11 +56459,11 @@
       <c r="J55" s="106"/>
       <c r="K55" s="178"/>
       <c r="L55" s="107"/>
-      <c r="M55" s="789"/>
-      <c r="N55" s="790"/>
-      <c r="O55" s="790"/>
-      <c r="P55" s="790"/>
-      <c r="Q55" s="791"/>
+      <c r="M55" s="778"/>
+      <c r="N55" s="779"/>
+      <c r="O55" s="779"/>
+      <c r="P55" s="779"/>
+      <c r="Q55" s="780"/>
     </row>
     <row r="56" spans="1:17" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
       <c r="C56" s="4" t="s">
@@ -56402,11 +56481,11 @@
         <v>15</v>
       </c>
       <c r="J56" s="109"/>
-      <c r="K56" s="760">
+      <c r="K56" s="771">
         <f>-C4</f>
         <v>-567389.35</v>
       </c>
-      <c r="L56" s="761"/>
+      <c r="L56" s="772"/>
     </row>
     <row r="57" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="110" t="s">
@@ -56423,22 +56502,22 @@
       <c r="C58" s="112">
         <v>44535</v>
       </c>
-      <c r="D58" s="738" t="s">
+      <c r="D58" s="749" t="s">
         <v>18</v>
       </c>
-      <c r="E58" s="739"/>
+      <c r="E58" s="750"/>
       <c r="F58" s="113">
         <v>2142307.62</v>
       </c>
-      <c r="I58" s="740" t="s">
+      <c r="I58" s="751" t="s">
         <v>198</v>
       </c>
-      <c r="J58" s="741"/>
-      <c r="K58" s="742">
+      <c r="J58" s="752"/>
+      <c r="K58" s="753">
         <f>K54+K56</f>
         <v>741389.00000000035</v>
       </c>
-      <c r="L58" s="742"/>
+      <c r="L58" s="753"/>
     </row>
     <row r="59" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C59" s="114"/>
@@ -56582,17 +56661,14 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="M54:Q55"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="M36:M37"/>
-    <mergeCell ref="N36:N37"/>
-    <mergeCell ref="Q36:Q37"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="W4:X5"/>
+    <mergeCell ref="W27:X28"/>
+    <mergeCell ref="Y27:Y28"/>
+    <mergeCell ref="W19:W20"/>
+    <mergeCell ref="W21:X21"/>
+    <mergeCell ref="W23:X24"/>
+    <mergeCell ref="W25:X25"/>
+    <mergeCell ref="W26:X26"/>
     <mergeCell ref="D58:E58"/>
     <mergeCell ref="I58:J58"/>
     <mergeCell ref="K58:L58"/>
@@ -56603,14 +56679,17 @@
     <mergeCell ref="I54:J54"/>
     <mergeCell ref="K54:L54"/>
     <mergeCell ref="K56:L56"/>
-    <mergeCell ref="W4:X5"/>
-    <mergeCell ref="W27:X28"/>
-    <mergeCell ref="Y27:Y28"/>
-    <mergeCell ref="W19:W20"/>
-    <mergeCell ref="W21:X21"/>
-    <mergeCell ref="W23:X24"/>
-    <mergeCell ref="W25:X25"/>
-    <mergeCell ref="W26:X26"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="M54:Q55"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="M36:M37"/>
+    <mergeCell ref="N36:N37"/>
+    <mergeCell ref="Q36:Q37"/>
   </mergeCells>
   <pageMargins left="0.15748031496062992" right="0.15748031496062992" top="0.27559055118110237" bottom="0.27559055118110237" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="68" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -59353,23 +59432,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="762"/>
-      <c r="C1" s="764" t="s">
+      <c r="B1" s="738"/>
+      <c r="C1" s="740" t="s">
         <v>208</v>
       </c>
-      <c r="D1" s="765"/>
-      <c r="E1" s="765"/>
-      <c r="F1" s="765"/>
-      <c r="G1" s="765"/>
-      <c r="H1" s="765"/>
-      <c r="I1" s="765"/>
-      <c r="J1" s="765"/>
-      <c r="K1" s="765"/>
-      <c r="L1" s="765"/>
-      <c r="M1" s="765"/>
+      <c r="D1" s="741"/>
+      <c r="E1" s="741"/>
+      <c r="F1" s="741"/>
+      <c r="G1" s="741"/>
+      <c r="H1" s="741"/>
+      <c r="I1" s="741"/>
+      <c r="J1" s="741"/>
+      <c r="K1" s="741"/>
+      <c r="L1" s="741"/>
+      <c r="M1" s="741"/>
     </row>
     <row r="2" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="763"/>
+      <c r="B2" s="739"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -59379,21 +59458,21 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:25" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="766" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="767"/>
+      <c r="B3" s="742" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="743"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="768" t="s">
+      <c r="H3" s="744" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="768"/>
+      <c r="I3" s="744"/>
       <c r="K3" s="165"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
-      <c r="P3" s="792" t="s">
+      <c r="P3" s="781" t="s">
         <v>6</v>
       </c>
       <c r="R3" s="802" t="s">
@@ -59411,14 +59490,14 @@
       <c r="D4" s="18">
         <v>44507</v>
       </c>
-      <c r="E4" s="769" t="s">
+      <c r="E4" s="745" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="770"/>
-      <c r="H4" s="771" t="s">
+      <c r="F4" s="746"/>
+      <c r="H4" s="747" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="772"/>
+      <c r="I4" s="748"/>
       <c r="J4" s="19"/>
       <c r="K4" s="166"/>
       <c r="L4" s="20"/>
@@ -59428,15 +59507,15 @@
       <c r="N4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="793"/>
+      <c r="P4" s="782"/>
       <c r="Q4" s="322" t="s">
         <v>217</v>
       </c>
       <c r="R4" s="803"/>
-      <c r="W4" s="775" t="s">
+      <c r="W4" s="791" t="s">
         <v>124</v>
       </c>
-      <c r="X4" s="775"/>
+      <c r="X4" s="791"/>
       <c r="Y4" s="227"/>
     </row>
     <row r="5" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -59497,8 +59576,8 @@
       <c r="S5" s="324" t="s">
         <v>213</v>
       </c>
-      <c r="W5" s="775"/>
-      <c r="X5" s="775"/>
+      <c r="W5" s="791"/>
+      <c r="X5" s="791"/>
       <c r="Y5" s="233"/>
     </row>
     <row r="6" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -60255,7 +60334,7 @@
         <v>0</v>
       </c>
       <c r="S19" s="147"/>
-      <c r="W19" s="779">
+      <c r="W19" s="795">
         <f>SUM(W6:W18)</f>
         <v>0</v>
       </c>
@@ -60307,7 +60386,7 @@
         <v>0</v>
       </c>
       <c r="S20" s="147"/>
-      <c r="W20" s="780"/>
+      <c r="W20" s="796"/>
       <c r="X20" s="268"/>
       <c r="Y20" s="233"/>
     </row>
@@ -60356,8 +60435,8 @@
         <v>0</v>
       </c>
       <c r="S21" s="147"/>
-      <c r="W21" s="781"/>
-      <c r="X21" s="781"/>
+      <c r="W21" s="797"/>
+      <c r="X21" s="797"/>
       <c r="Y21" s="233"/>
       <c r="Z21" s="128"/>
     </row>
@@ -60458,8 +60537,8 @@
         <v>0</v>
       </c>
       <c r="S23" s="147"/>
-      <c r="W23" s="782"/>
-      <c r="X23" s="782"/>
+      <c r="W23" s="798"/>
+      <c r="X23" s="798"/>
       <c r="Y23" s="233"/>
       <c r="Z23" s="128"/>
     </row>
@@ -60510,8 +60589,8 @@
         <v>0</v>
       </c>
       <c r="S24" s="147"/>
-      <c r="W24" s="782"/>
-      <c r="X24" s="782"/>
+      <c r="W24" s="798"/>
+      <c r="X24" s="798"/>
       <c r="Y24" s="233"/>
       <c r="Z24" s="128"/>
     </row>
@@ -60557,8 +60636,8 @@
       <c r="R25" s="319">
         <v>0</v>
       </c>
-      <c r="W25" s="783"/>
-      <c r="X25" s="783"/>
+      <c r="W25" s="799"/>
+      <c r="X25" s="799"/>
       <c r="Y25" s="233"/>
       <c r="Z25" s="128"/>
     </row>
@@ -60606,8 +60685,8 @@
       <c r="R26" s="319">
         <v>0</v>
       </c>
-      <c r="W26" s="783"/>
-      <c r="X26" s="783"/>
+      <c r="W26" s="799"/>
+      <c r="X26" s="799"/>
       <c r="Y26" s="233"/>
       <c r="Z26" s="128"/>
     </row>
@@ -60667,9 +60746,9 @@
       <c r="V27" t="s">
         <v>240</v>
       </c>
-      <c r="W27" s="776"/>
-      <c r="X27" s="777"/>
-      <c r="Y27" s="778"/>
+      <c r="W27" s="792"/>
+      <c r="X27" s="793"/>
+      <c r="Y27" s="794"/>
       <c r="Z27" s="128"/>
     </row>
     <row r="28" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -60723,9 +60802,9 @@
       <c r="V28" t="s">
         <v>240</v>
       </c>
-      <c r="W28" s="777"/>
-      <c r="X28" s="777"/>
-      <c r="Y28" s="778"/>
+      <c r="W28" s="793"/>
+      <c r="X28" s="793"/>
+      <c r="Y28" s="794"/>
       <c r="Z28" s="128"/>
     </row>
     <row r="29" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -61041,11 +61120,11 @@
       <c r="J36" s="266"/>
       <c r="K36" s="250"/>
       <c r="L36" s="44"/>
-      <c r="M36" s="794">
+      <c r="M36" s="783">
         <f>SUM(M5:M35)</f>
         <v>1077791.3</v>
       </c>
-      <c r="N36" s="796">
+      <c r="N36" s="785">
         <f>SUM(N5:N35)</f>
         <v>936398</v>
       </c>
@@ -61053,7 +61132,7 @@
       <c r="P36" s="277">
         <v>0</v>
       </c>
-      <c r="Q36" s="798">
+      <c r="Q36" s="787">
         <f>SUM(Q5:Q35)</f>
         <v>-14262.940000000002</v>
       </c>
@@ -61072,13 +61151,13 @@
       <c r="J37" s="60"/>
       <c r="K37" s="41"/>
       <c r="L37" s="61"/>
-      <c r="M37" s="795"/>
-      <c r="N37" s="797"/>
+      <c r="M37" s="784"/>
+      <c r="N37" s="786"/>
       <c r="O37" s="276"/>
       <c r="P37" s="277">
         <v>0</v>
       </c>
-      <c r="Q37" s="799"/>
+      <c r="Q37" s="788"/>
     </row>
     <row r="38" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="23"/>
@@ -61352,26 +61431,26 @@
       <c r="A52" s="98"/>
       <c r="B52" s="99"/>
       <c r="C52" s="1"/>
-      <c r="H52" s="749" t="s">
+      <c r="H52" s="760" t="s">
         <v>11</v>
       </c>
-      <c r="I52" s="750"/>
+      <c r="I52" s="761"/>
       <c r="J52" s="100"/>
-      <c r="K52" s="751">
+      <c r="K52" s="762">
         <f>I50+L50</f>
         <v>90750.75</v>
       </c>
-      <c r="L52" s="784"/>
+      <c r="L52" s="789"/>
       <c r="M52" s="272"/>
       <c r="N52" s="272"/>
       <c r="P52" s="34"/>
       <c r="Q52" s="13"/>
     </row>
     <row r="53" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D53" s="755" t="s">
+      <c r="D53" s="766" t="s">
         <v>12</v>
       </c>
-      <c r="E53" s="755"/>
+      <c r="E53" s="766"/>
       <c r="F53" s="312">
         <f>F50-K52-C50</f>
         <v>1739855.03</v>
@@ -61380,29 +61459,29 @@
       <c r="J53" s="103"/>
     </row>
     <row r="54" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D54" s="785" t="s">
+      <c r="D54" s="790" t="s">
         <v>95</v>
       </c>
-      <c r="E54" s="785"/>
+      <c r="E54" s="790"/>
       <c r="F54" s="111">
         <v>-1567070.66</v>
       </c>
-      <c r="I54" s="756" t="s">
+      <c r="I54" s="767" t="s">
         <v>13</v>
       </c>
-      <c r="J54" s="757"/>
-      <c r="K54" s="758">
+      <c r="J54" s="768"/>
+      <c r="K54" s="769">
         <f>F56+F57+F58</f>
         <v>703192.8600000001</v>
       </c>
-      <c r="L54" s="758"/>
-      <c r="M54" s="786" t="s">
+      <c r="L54" s="769"/>
+      <c r="M54" s="775" t="s">
         <v>211</v>
       </c>
-      <c r="N54" s="787"/>
-      <c r="O54" s="787"/>
-      <c r="P54" s="787"/>
-      <c r="Q54" s="788"/>
+      <c r="N54" s="776"/>
+      <c r="O54" s="776"/>
+      <c r="P54" s="776"/>
+      <c r="Q54" s="777"/>
     </row>
     <row r="55" spans="1:17" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D55" s="313" t="s">
@@ -61416,11 +61495,11 @@
       <c r="J55" s="106"/>
       <c r="K55" s="178"/>
       <c r="L55" s="107"/>
-      <c r="M55" s="789"/>
-      <c r="N55" s="790"/>
-      <c r="O55" s="790"/>
-      <c r="P55" s="790"/>
-      <c r="Q55" s="791"/>
+      <c r="M55" s="778"/>
+      <c r="N55" s="779"/>
+      <c r="O55" s="779"/>
+      <c r="P55" s="779"/>
+      <c r="Q55" s="780"/>
     </row>
     <row r="56" spans="1:17" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
       <c r="C56" s="4" t="s">
@@ -61438,11 +61517,11 @@
         <v>15</v>
       </c>
       <c r="J56" s="109"/>
-      <c r="K56" s="760">
+      <c r="K56" s="771">
         <f>-C4</f>
         <v>-567389.35</v>
       </c>
-      <c r="L56" s="761"/>
+      <c r="L56" s="772"/>
     </row>
     <row r="57" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="110" t="s">
@@ -61459,22 +61538,22 @@
       <c r="C58" s="112">
         <v>44563</v>
       </c>
-      <c r="D58" s="738" t="s">
+      <c r="D58" s="749" t="s">
         <v>18</v>
       </c>
-      <c r="E58" s="739"/>
+      <c r="E58" s="750"/>
       <c r="F58" s="113">
         <v>754143.23</v>
       </c>
-      <c r="I58" s="740" t="s">
+      <c r="I58" s="751" t="s">
         <v>198</v>
       </c>
-      <c r="J58" s="741"/>
-      <c r="K58" s="742">
+      <c r="J58" s="752"/>
+      <c r="K58" s="753">
         <f>K54+K56</f>
         <v>135803.51000000013</v>
       </c>
-      <c r="L58" s="742"/>
+      <c r="L58" s="753"/>
     </row>
     <row r="59" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C59" s="114"/>
@@ -61618,13 +61697,20 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="D58:E58"/>
+    <mergeCell ref="I58:J58"/>
+    <mergeCell ref="K58:L58"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="D54:E54"/>
+    <mergeCell ref="I54:J54"/>
+    <mergeCell ref="K54:L54"/>
+    <mergeCell ref="M54:Q55"/>
+    <mergeCell ref="K56:L56"/>
+    <mergeCell ref="W27:X28"/>
+    <mergeCell ref="Y27:Y28"/>
+    <mergeCell ref="M36:M37"/>
+    <mergeCell ref="N36:N37"/>
+    <mergeCell ref="Q36:Q37"/>
     <mergeCell ref="H52:I52"/>
     <mergeCell ref="K52:L52"/>
     <mergeCell ref="W4:X5"/>
@@ -61634,20 +61720,13 @@
     <mergeCell ref="W25:X25"/>
     <mergeCell ref="W26:X26"/>
     <mergeCell ref="R3:R4"/>
-    <mergeCell ref="M54:Q55"/>
-    <mergeCell ref="K56:L56"/>
-    <mergeCell ref="W27:X28"/>
-    <mergeCell ref="Y27:Y28"/>
-    <mergeCell ref="M36:M37"/>
-    <mergeCell ref="N36:N37"/>
-    <mergeCell ref="Q36:Q37"/>
-    <mergeCell ref="D58:E58"/>
-    <mergeCell ref="I58:J58"/>
-    <mergeCell ref="K58:L58"/>
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="D54:E54"/>
-    <mergeCell ref="I54:J54"/>
-    <mergeCell ref="K54:L54"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -64342,7 +64421,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="762"/>
+      <c r="B1" s="738"/>
       <c r="C1" s="804" t="s">
         <v>316</v>
       </c>
@@ -64358,7 +64437,7 @@
       <c r="M1" s="805"/>
     </row>
     <row r="2" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="763"/>
+      <c r="B2" s="739"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -64368,21 +64447,21 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:25" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="766" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="767"/>
+      <c r="B3" s="742" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="743"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="768" t="s">
+      <c r="H3" s="744" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="768"/>
+      <c r="I3" s="744"/>
       <c r="K3" s="165"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
-      <c r="P3" s="792" t="s">
+      <c r="P3" s="781" t="s">
         <v>6</v>
       </c>
       <c r="R3" s="802" t="s">
@@ -64400,14 +64479,14 @@
       <c r="D4" s="18">
         <v>44563</v>
       </c>
-      <c r="E4" s="769" t="s">
+      <c r="E4" s="745" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="770"/>
-      <c r="H4" s="771" t="s">
+      <c r="F4" s="746"/>
+      <c r="H4" s="747" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="772"/>
+      <c r="I4" s="748"/>
       <c r="J4" s="19"/>
       <c r="K4" s="166"/>
       <c r="L4" s="20"/>
@@ -64417,15 +64496,15 @@
       <c r="N4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="793"/>
+      <c r="P4" s="782"/>
       <c r="Q4" s="322" t="s">
         <v>217</v>
       </c>
       <c r="R4" s="803"/>
-      <c r="W4" s="775" t="s">
+      <c r="W4" s="791" t="s">
         <v>124</v>
       </c>
-      <c r="X4" s="775"/>
+      <c r="X4" s="791"/>
       <c r="Y4" s="227"/>
     </row>
     <row r="5" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -64476,8 +64555,8 @@
         <v>0</v>
       </c>
       <c r="S5" s="324"/>
-      <c r="W5" s="775"/>
-      <c r="X5" s="775"/>
+      <c r="W5" s="791"/>
+      <c r="X5" s="791"/>
       <c r="Y5" s="233"/>
     </row>
     <row r="6" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -65241,7 +65320,7 @@
         <v>0</v>
       </c>
       <c r="S19" s="147"/>
-      <c r="W19" s="779">
+      <c r="W19" s="795">
         <f>SUM(W6:W18)</f>
         <v>0</v>
       </c>
@@ -65294,7 +65373,7 @@
         <v>0</v>
       </c>
       <c r="S20" s="147"/>
-      <c r="W20" s="780"/>
+      <c r="W20" s="796"/>
       <c r="X20" s="268"/>
       <c r="Y20" s="233"/>
     </row>
@@ -65343,8 +65422,8 @@
         <v>377273.87</v>
       </c>
       <c r="S21" s="147"/>
-      <c r="W21" s="781"/>
-      <c r="X21" s="781"/>
+      <c r="W21" s="797"/>
+      <c r="X21" s="797"/>
       <c r="Y21" s="233"/>
       <c r="Z21" s="128"/>
     </row>
@@ -65444,8 +65523,8 @@
         <v>0</v>
       </c>
       <c r="S23" s="147"/>
-      <c r="W23" s="782"/>
-      <c r="X23" s="782"/>
+      <c r="W23" s="798"/>
+      <c r="X23" s="798"/>
       <c r="Y23" s="233"/>
       <c r="Z23" s="128"/>
     </row>
@@ -65500,8 +65579,8 @@
         <v>0</v>
       </c>
       <c r="S24" s="147"/>
-      <c r="W24" s="782"/>
-      <c r="X24" s="782"/>
+      <c r="W24" s="798"/>
+      <c r="X24" s="798"/>
       <c r="Y24" s="233"/>
       <c r="Z24" s="128"/>
     </row>
@@ -65546,8 +65625,8 @@
       <c r="R25" s="319">
         <v>0</v>
       </c>
-      <c r="W25" s="783"/>
-      <c r="X25" s="783"/>
+      <c r="W25" s="799"/>
+      <c r="X25" s="799"/>
       <c r="Y25" s="233"/>
       <c r="Z25" s="128"/>
     </row>
@@ -65595,8 +65674,8 @@
       <c r="R26" s="319">
         <v>0</v>
       </c>
-      <c r="W26" s="783"/>
-      <c r="X26" s="783"/>
+      <c r="W26" s="799"/>
+      <c r="X26" s="799"/>
       <c r="Y26" s="233"/>
       <c r="Z26" s="128"/>
     </row>
@@ -65650,9 +65729,9 @@
       <c r="V27" t="s">
         <v>240</v>
       </c>
-      <c r="W27" s="776"/>
-      <c r="X27" s="777"/>
-      <c r="Y27" s="778"/>
+      <c r="W27" s="792"/>
+      <c r="X27" s="793"/>
+      <c r="Y27" s="794"/>
       <c r="Z27" s="128"/>
     </row>
     <row r="28" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -65706,9 +65785,9 @@
       <c r="V28" t="s">
         <v>240</v>
       </c>
-      <c r="W28" s="777"/>
-      <c r="X28" s="777"/>
-      <c r="Y28" s="778"/>
+      <c r="W28" s="793"/>
+      <c r="X28" s="793"/>
+      <c r="Y28" s="794"/>
       <c r="Z28" s="128"/>
     </row>
     <row r="29" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -66019,11 +66098,11 @@
       <c r="L36" s="44">
         <v>13275.84</v>
       </c>
-      <c r="M36" s="794">
+      <c r="M36" s="783">
         <f>SUM(M5:M35)</f>
         <v>1818445.73</v>
       </c>
-      <c r="N36" s="796">
+      <c r="N36" s="785">
         <f>SUM(N5:N35)</f>
         <v>739014</v>
       </c>
@@ -66031,7 +66110,7 @@
       <c r="P36" s="277">
         <v>0</v>
       </c>
-      <c r="Q36" s="798">
+      <c r="Q36" s="787">
         <f>SUM(Q5:Q35)</f>
         <v>-7.2800000000133878</v>
       </c>
@@ -66056,13 +66135,13 @@
       <c r="L37" s="61">
         <v>15060.32</v>
       </c>
-      <c r="M37" s="795"/>
-      <c r="N37" s="797"/>
+      <c r="M37" s="784"/>
+      <c r="N37" s="786"/>
       <c r="O37" s="276"/>
       <c r="P37" s="277">
         <v>0</v>
       </c>
-      <c r="Q37" s="799"/>
+      <c r="Q37" s="788"/>
       <c r="R37" s="227" t="s">
         <v>7</v>
       </c>
@@ -66355,26 +66434,26 @@
       <c r="A52" s="98"/>
       <c r="B52" s="99"/>
       <c r="C52" s="1"/>
-      <c r="H52" s="749" t="s">
+      <c r="H52" s="760" t="s">
         <v>11</v>
       </c>
-      <c r="I52" s="750"/>
+      <c r="I52" s="761"/>
       <c r="J52" s="100"/>
-      <c r="K52" s="751">
+      <c r="K52" s="762">
         <f>I50+L50</f>
         <v>158798.12</v>
       </c>
-      <c r="L52" s="784"/>
+      <c r="L52" s="789"/>
       <c r="M52" s="272"/>
       <c r="N52" s="272"/>
       <c r="P52" s="34"/>
       <c r="Q52" s="13"/>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D53" s="755" t="s">
+      <c r="D53" s="766" t="s">
         <v>12</v>
       </c>
-      <c r="E53" s="755"/>
+      <c r="E53" s="766"/>
       <c r="F53" s="312">
         <f>F50-K52-C50</f>
         <v>2078470.75</v>
@@ -66383,22 +66462,22 @@
       <c r="J53" s="103"/>
     </row>
     <row r="54" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D54" s="785" t="s">
+      <c r="D54" s="790" t="s">
         <v>95</v>
       </c>
-      <c r="E54" s="785"/>
+      <c r="E54" s="790"/>
       <c r="F54" s="111">
         <v>-1448401.2</v>
       </c>
-      <c r="I54" s="756" t="s">
+      <c r="I54" s="767" t="s">
         <v>13</v>
       </c>
-      <c r="J54" s="757"/>
-      <c r="K54" s="758">
+      <c r="J54" s="768"/>
+      <c r="K54" s="769">
         <f>F56+F57+F58</f>
         <v>1025960.7</v>
       </c>
-      <c r="L54" s="758"/>
+      <c r="L54" s="769"/>
       <c r="M54" s="404"/>
       <c r="N54" s="404"/>
       <c r="O54" s="404"/>
@@ -66439,11 +66518,11 @@
         <v>15</v>
       </c>
       <c r="J56" s="109"/>
-      <c r="K56" s="760">
+      <c r="K56" s="771">
         <f>-C4</f>
         <v>-754143.23</v>
       </c>
-      <c r="L56" s="761"/>
+      <c r="L56" s="772"/>
     </row>
     <row r="57" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="110" t="s">
@@ -66460,22 +66539,22 @@
       <c r="C58" s="112">
         <v>44591</v>
       </c>
-      <c r="D58" s="738" t="s">
+      <c r="D58" s="749" t="s">
         <v>18</v>
       </c>
-      <c r="E58" s="739"/>
+      <c r="E58" s="750"/>
       <c r="F58" s="113">
         <v>1149740.4099999999</v>
       </c>
-      <c r="I58" s="740" t="s">
+      <c r="I58" s="751" t="s">
         <v>198</v>
       </c>
-      <c r="J58" s="741"/>
-      <c r="K58" s="742">
+      <c r="J58" s="752"/>
+      <c r="K58" s="753">
         <f>K54+K56</f>
         <v>271817.46999999997</v>
       </c>
-      <c r="L58" s="742"/>
+      <c r="L58" s="753"/>
     </row>
     <row r="59" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C59" s="114"/>
@@ -66619,6 +66698,20 @@
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="Y27:Y28"/>
+    <mergeCell ref="M36:M37"/>
+    <mergeCell ref="N36:N37"/>
+    <mergeCell ref="Q36:Q37"/>
+    <mergeCell ref="D58:E58"/>
+    <mergeCell ref="I58:J58"/>
+    <mergeCell ref="K58:L58"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="D54:E54"/>
+    <mergeCell ref="I54:J54"/>
+    <mergeCell ref="K54:L54"/>
+    <mergeCell ref="K56:L56"/>
+    <mergeCell ref="H52:I52"/>
+    <mergeCell ref="K52:L52"/>
     <mergeCell ref="W26:X26"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="W27:X28"/>
@@ -66634,20 +66727,6 @@
     <mergeCell ref="W21:X21"/>
     <mergeCell ref="W23:X24"/>
     <mergeCell ref="W25:X25"/>
-    <mergeCell ref="Y27:Y28"/>
-    <mergeCell ref="M36:M37"/>
-    <mergeCell ref="N36:N37"/>
-    <mergeCell ref="Q36:Q37"/>
-    <mergeCell ref="D58:E58"/>
-    <mergeCell ref="I58:J58"/>
-    <mergeCell ref="K58:L58"/>
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="D54:E54"/>
-    <mergeCell ref="I54:J54"/>
-    <mergeCell ref="K54:L54"/>
-    <mergeCell ref="K56:L56"/>
-    <mergeCell ref="H52:I52"/>
-    <mergeCell ref="K52:L52"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -69441,7 +69520,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="762"/>
+      <c r="B1" s="738"/>
       <c r="C1" s="804" t="s">
         <v>646</v>
       </c>
@@ -69457,7 +69536,7 @@
       <c r="M1" s="805"/>
     </row>
     <row r="2" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="763"/>
+      <c r="B2" s="739"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -69467,21 +69546,21 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:25" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="766" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="767"/>
+      <c r="B3" s="742" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="743"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="768" t="s">
+      <c r="H3" s="744" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="768"/>
+      <c r="I3" s="744"/>
       <c r="K3" s="165"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
-      <c r="P3" s="792" t="s">
+      <c r="P3" s="781" t="s">
         <v>6</v>
       </c>
       <c r="R3" s="802" t="s">
@@ -69499,14 +69578,14 @@
       <c r="D4" s="18">
         <v>44591</v>
       </c>
-      <c r="E4" s="769" t="s">
+      <c r="E4" s="745" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="770"/>
-      <c r="H4" s="771" t="s">
+      <c r="F4" s="746"/>
+      <c r="H4" s="747" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="772"/>
+      <c r="I4" s="748"/>
       <c r="J4" s="19"/>
       <c r="K4" s="166"/>
       <c r="L4" s="20"/>
@@ -69516,15 +69595,15 @@
       <c r="N4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="793"/>
+      <c r="P4" s="782"/>
       <c r="Q4" s="322" t="s">
         <v>217</v>
       </c>
       <c r="R4" s="803"/>
-      <c r="W4" s="775" t="s">
+      <c r="W4" s="791" t="s">
         <v>124</v>
       </c>
-      <c r="X4" s="775"/>
+      <c r="X4" s="791"/>
       <c r="Y4" s="227"/>
     </row>
     <row r="5" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -69575,8 +69654,8 @@
         <v>0</v>
       </c>
       <c r="S5" s="324"/>
-      <c r="W5" s="775"/>
-      <c r="X5" s="775"/>
+      <c r="W5" s="791"/>
+      <c r="X5" s="791"/>
       <c r="Y5" s="233"/>
     </row>
     <row r="6" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -70337,7 +70416,7 @@
         <v>0</v>
       </c>
       <c r="S19" s="147"/>
-      <c r="W19" s="779">
+      <c r="W19" s="795">
         <f>SUM(W6:W18)</f>
         <v>0</v>
       </c>
@@ -70389,7 +70468,7 @@
         <v>0</v>
       </c>
       <c r="S20" s="147"/>
-      <c r="W20" s="780"/>
+      <c r="W20" s="796"/>
       <c r="X20" s="268"/>
       <c r="Y20" s="233"/>
     </row>
@@ -70438,8 +70517,8 @@
         <v>18072</v>
       </c>
       <c r="S21" s="147"/>
-      <c r="W21" s="781"/>
-      <c r="X21" s="781"/>
+      <c r="W21" s="797"/>
+      <c r="X21" s="797"/>
       <c r="Y21" s="233"/>
       <c r="Z21" s="128"/>
     </row>
@@ -70538,8 +70617,8 @@
         <v>0</v>
       </c>
       <c r="S23" s="147"/>
-      <c r="W23" s="782"/>
-      <c r="X23" s="782"/>
+      <c r="W23" s="798"/>
+      <c r="X23" s="798"/>
       <c r="Y23" s="233"/>
       <c r="Z23" s="128"/>
     </row>
@@ -70594,8 +70673,8 @@
         <v>0</v>
       </c>
       <c r="S24" s="147"/>
-      <c r="W24" s="782"/>
-      <c r="X24" s="782"/>
+      <c r="W24" s="798"/>
+      <c r="X24" s="798"/>
       <c r="Y24" s="233"/>
       <c r="Z24" s="128"/>
     </row>
@@ -70643,8 +70722,8 @@
       <c r="R25" s="319">
         <v>0</v>
       </c>
-      <c r="W25" s="783"/>
-      <c r="X25" s="783"/>
+      <c r="W25" s="799"/>
+      <c r="X25" s="799"/>
       <c r="Y25" s="233"/>
       <c r="Z25" s="128"/>
     </row>
@@ -70692,8 +70771,8 @@
       <c r="R26" s="319">
         <v>0</v>
       </c>
-      <c r="W26" s="783"/>
-      <c r="X26" s="783"/>
+      <c r="W26" s="799"/>
+      <c r="X26" s="799"/>
       <c r="Y26" s="233"/>
       <c r="Z26" s="128"/>
     </row>
@@ -70741,9 +70820,9 @@
       <c r="R27" s="319">
         <v>0</v>
       </c>
-      <c r="W27" s="776"/>
-      <c r="X27" s="777"/>
-      <c r="Y27" s="778"/>
+      <c r="W27" s="792"/>
+      <c r="X27" s="793"/>
+      <c r="Y27" s="794"/>
       <c r="Z27" s="128"/>
     </row>
     <row r="28" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -70791,9 +70870,9 @@
       <c r="R28" s="319">
         <v>0</v>
       </c>
-      <c r="W28" s="777"/>
-      <c r="X28" s="777"/>
-      <c r="Y28" s="778"/>
+      <c r="W28" s="793"/>
+      <c r="X28" s="793"/>
+      <c r="Y28" s="794"/>
       <c r="Z28" s="128"/>
     </row>
     <row r="29" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -71134,11 +71213,11 @@
       <c r="J36" s="266"/>
       <c r="K36" s="250"/>
       <c r="L36" s="44"/>
-      <c r="M36" s="794">
+      <c r="M36" s="783">
         <f>SUM(M5:M35)</f>
         <v>2143864.4900000002</v>
       </c>
-      <c r="N36" s="796">
+      <c r="N36" s="785">
         <f>SUM(N5:N35)</f>
         <v>791108</v>
       </c>
@@ -71171,8 +71250,8 @@
       <c r="L37" s="61">
         <v>16518.78</v>
       </c>
-      <c r="M37" s="795"/>
-      <c r="N37" s="797"/>
+      <c r="M37" s="784"/>
+      <c r="N37" s="786"/>
       <c r="O37" s="276"/>
       <c r="P37" s="277">
         <v>0</v>
@@ -71479,26 +71558,26 @@
       <c r="A52" s="98"/>
       <c r="B52" s="99"/>
       <c r="C52" s="1"/>
-      <c r="H52" s="749" t="s">
+      <c r="H52" s="760" t="s">
         <v>11</v>
       </c>
-      <c r="I52" s="750"/>
+      <c r="I52" s="761"/>
       <c r="J52" s="100"/>
-      <c r="K52" s="751">
+      <c r="K52" s="762">
         <f>I50+L50</f>
         <v>197471.8</v>
       </c>
-      <c r="L52" s="784"/>
+      <c r="L52" s="789"/>
       <c r="M52" s="272"/>
       <c r="N52" s="272"/>
       <c r="P52" s="34"/>
       <c r="Q52" s="13"/>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D53" s="755" t="s">
+      <c r="D53" s="766" t="s">
         <v>12</v>
       </c>
-      <c r="E53" s="755"/>
+      <c r="E53" s="766"/>
       <c r="F53" s="312">
         <f>F50-K52-C50</f>
         <v>2057786.11</v>
@@ -71507,22 +71586,22 @@
       <c r="J53" s="103"/>
     </row>
     <row r="54" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D54" s="785" t="s">
+      <c r="D54" s="790" t="s">
         <v>95</v>
       </c>
-      <c r="E54" s="785"/>
+      <c r="E54" s="790"/>
       <c r="F54" s="111">
         <v>-1702928.14</v>
       </c>
-      <c r="I54" s="756" t="s">
+      <c r="I54" s="767" t="s">
         <v>13</v>
       </c>
-      <c r="J54" s="757"/>
-      <c r="K54" s="758">
+      <c r="J54" s="768"/>
+      <c r="K54" s="769">
         <f>F56+F57+F58</f>
         <v>1147965.3400000003</v>
       </c>
-      <c r="L54" s="758"/>
+      <c r="L54" s="769"/>
       <c r="M54" s="404"/>
       <c r="N54" s="404"/>
       <c r="O54" s="404"/>
@@ -71563,11 +71642,11 @@
         <v>15</v>
       </c>
       <c r="J56" s="109"/>
-      <c r="K56" s="760">
+      <c r="K56" s="771">
         <f>-C4</f>
         <v>-1149740.4099999999</v>
       </c>
-      <c r="L56" s="761"/>
+      <c r="L56" s="772"/>
     </row>
     <row r="57" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="110" t="s">
@@ -71584,22 +71663,22 @@
       <c r="C58" s="112">
         <v>44619</v>
       </c>
-      <c r="D58" s="738" t="s">
+      <c r="D58" s="749" t="s">
         <v>18</v>
       </c>
-      <c r="E58" s="739"/>
+      <c r="E58" s="750"/>
       <c r="F58" s="113">
         <v>1266568.45</v>
       </c>
-      <c r="I58" s="740" t="s">
+      <c r="I58" s="751" t="s">
         <v>97</v>
       </c>
-      <c r="J58" s="741"/>
-      <c r="K58" s="742">
+      <c r="J58" s="752"/>
+      <c r="K58" s="753">
         <f>K54+K56</f>
         <v>-1775.0699999995995</v>
       </c>
-      <c r="L58" s="742"/>
+      <c r="L58" s="753"/>
     </row>
     <row r="59" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C59" s="114"/>
@@ -71743,20 +71822,6 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="W26:X26"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="R3:R4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="W4:X5"/>
-    <mergeCell ref="W19:W20"/>
-    <mergeCell ref="W21:X21"/>
-    <mergeCell ref="W23:X24"/>
-    <mergeCell ref="W25:X25"/>
     <mergeCell ref="D58:E58"/>
     <mergeCell ref="I58:J58"/>
     <mergeCell ref="K58:L58"/>
@@ -71773,6 +71838,20 @@
     <mergeCell ref="K54:L54"/>
     <mergeCell ref="K56:L56"/>
     <mergeCell ref="M39:N39"/>
+    <mergeCell ref="W26:X26"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="R3:R4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="W4:X5"/>
+    <mergeCell ref="W19:W20"/>
+    <mergeCell ref="W21:X21"/>
+    <mergeCell ref="W23:X24"/>
+    <mergeCell ref="W25:X25"/>
   </mergeCells>
   <pageMargins left="0.23" right="0.23" top="0.4" bottom="0.28000000000000003" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>